<commit_message>
Added a new control.
</commit_message>
<xml_diff>
--- a/Controls.xlsx
+++ b/Controls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl-Otto\Documents\src\NVDA\vismaadministration-nvdaaddon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1B2C1F-EBCD-4FB0-B40C-71C2F0BF6618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2553B51-9FB9-4109-8C90-BFBAB8DE9B75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="30915" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="23040" windowHeight="12232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="302">
   <si>
     <t>WindowClassName</t>
   </si>
@@ -955,6 +955,12 @@
   </si>
   <si>
     <t>spcsfor</t>
+  </si>
+  <si>
+    <t>Anteckningar</t>
+  </si>
+  <si>
+    <t>Inställningar för egen kopia, utskriftsval</t>
   </si>
 </sst>
 </file>
@@ -1272,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E331"/>
+  <dimension ref="A1:E333"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A306" workbookViewId="0">
+      <selection activeCell="D333" sqref="D333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1934,13 +1940,10 @@
         <v>7</v>
       </c>
       <c r="B52">
-        <v>24279</v>
+        <v>20593</v>
       </c>
       <c r="D52" t="s">
-        <v>34</v>
-      </c>
-      <c r="E52" t="s">
-        <v>33</v>
+        <v>300</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
@@ -1948,10 +1951,13 @@
         <v>7</v>
       </c>
       <c r="B53">
-        <v>22642</v>
+        <v>24279</v>
       </c>
       <c r="D53" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="E53" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
@@ -1959,10 +1965,10 @@
         <v>7</v>
       </c>
       <c r="B54">
-        <v>22628</v>
+        <v>22642</v>
       </c>
       <c r="D54" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.45">
@@ -1970,10 +1976,10 @@
         <v>7</v>
       </c>
       <c r="B55">
-        <v>22629</v>
+        <v>22628</v>
       </c>
       <c r="D55" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.45">
@@ -1981,46 +1987,46 @@
         <v>7</v>
       </c>
       <c r="B56">
-        <v>22630</v>
+        <v>22629</v>
       </c>
       <c r="D56" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B57">
-        <v>22657</v>
+        <v>22630</v>
       </c>
       <c r="D57" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>7</v>
-      </c>
-      <c r="B58" t="s">
-        <v>41</v>
+        <v>20</v>
+      </c>
+      <c r="B58">
+        <v>22657</v>
       </c>
       <c r="D58" t="s">
-        <v>42</v>
-      </c>
-      <c r="E58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>7</v>
       </c>
-      <c r="B59">
-        <v>22631</v>
+      <c r="B59" t="s">
+        <v>41</v>
       </c>
       <c r="D59" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="E59" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.45">
@@ -2028,10 +2034,10 @@
         <v>7</v>
       </c>
       <c r="B60">
-        <v>22653</v>
+        <v>22631</v>
       </c>
       <c r="D60" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.45">
@@ -2039,10 +2045,10 @@
         <v>7</v>
       </c>
       <c r="B61">
-        <v>22654</v>
+        <v>22653</v>
       </c>
       <c r="D61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.45">
@@ -2050,10 +2056,10 @@
         <v>7</v>
       </c>
       <c r="B62">
-        <v>22655</v>
+        <v>22654</v>
       </c>
       <c r="D62" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.45">
@@ -2061,10 +2067,10 @@
         <v>7</v>
       </c>
       <c r="B63">
-        <v>22623</v>
+        <v>22655</v>
       </c>
       <c r="D63" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.45">
@@ -2072,10 +2078,10 @@
         <v>7</v>
       </c>
       <c r="B64">
-        <v>22625</v>
+        <v>22623</v>
       </c>
       <c r="D64" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.45">
@@ -2083,41 +2089,35 @@
         <v>7</v>
       </c>
       <c r="B65">
-        <v>22624</v>
+        <v>22625</v>
       </c>
       <c r="D65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B66">
-        <v>22673</v>
+        <v>22624</v>
       </c>
       <c r="D66" t="s">
-        <v>51</v>
-      </c>
-      <c r="E66" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B67">
-        <v>22308</v>
-      </c>
-      <c r="C67" t="s">
-        <v>225</v>
+        <v>22673</v>
       </c>
       <c r="D67" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E67" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.45">
@@ -2128,10 +2128,13 @@
         <v>22308</v>
       </c>
       <c r="C68" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D68" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="E68" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.45">
@@ -2142,7 +2145,10 @@
         <v>22308</v>
       </c>
       <c r="C69" t="s">
-        <v>227</v>
+        <v>226</v>
+      </c>
+      <c r="D69" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.45">
@@ -2150,10 +2156,10 @@
         <v>7</v>
       </c>
       <c r="B70">
-        <v>22332</v>
-      </c>
-      <c r="D70" t="s">
-        <v>55</v>
+        <v>22308</v>
+      </c>
+      <c r="C70" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.45">
@@ -2161,10 +2167,10 @@
         <v>7</v>
       </c>
       <c r="B71">
-        <v>22333</v>
+        <v>22332</v>
       </c>
       <c r="D71" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.45">
@@ -2172,10 +2178,10 @@
         <v>7</v>
       </c>
       <c r="B72">
-        <v>22344</v>
+        <v>22333</v>
       </c>
       <c r="D72" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.45">
@@ -2183,10 +2189,10 @@
         <v>7</v>
       </c>
       <c r="B73">
-        <v>22346</v>
+        <v>22344</v>
       </c>
       <c r="D73" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.45">
@@ -2194,10 +2200,10 @@
         <v>7</v>
       </c>
       <c r="B74">
-        <v>23613</v>
+        <v>22346</v>
       </c>
       <c r="D74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.45">
@@ -2205,10 +2211,10 @@
         <v>7</v>
       </c>
       <c r="B75">
-        <v>22362</v>
+        <v>23613</v>
       </c>
       <c r="D75" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.45">
@@ -2216,10 +2222,10 @@
         <v>7</v>
       </c>
       <c r="B76">
-        <v>22363</v>
+        <v>22362</v>
       </c>
       <c r="D76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.45">
@@ -2227,10 +2233,10 @@
         <v>7</v>
       </c>
       <c r="B77">
-        <v>22364</v>
+        <v>22363</v>
       </c>
       <c r="D77" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.45">
@@ -2238,10 +2244,10 @@
         <v>7</v>
       </c>
       <c r="B78">
-        <v>23658</v>
+        <v>22364</v>
       </c>
       <c r="D78" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.45">
@@ -2249,10 +2255,10 @@
         <v>7</v>
       </c>
       <c r="B79">
-        <v>22385</v>
+        <v>23658</v>
       </c>
       <c r="D79" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.45">
@@ -2260,10 +2266,10 @@
         <v>7</v>
       </c>
       <c r="B80">
-        <v>22384</v>
+        <v>22385</v>
       </c>
       <c r="D80" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.45">
@@ -2271,13 +2277,10 @@
         <v>7</v>
       </c>
       <c r="B81">
-        <v>22316</v>
-      </c>
-      <c r="C81" t="s">
-        <v>227</v>
+        <v>22384</v>
       </c>
       <c r="D81" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.45">
@@ -2288,10 +2291,10 @@
         <v>22316</v>
       </c>
       <c r="C82" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D82" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.45">
@@ -2302,10 +2305,10 @@
         <v>22316</v>
       </c>
       <c r="C83" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D83" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.45">
@@ -2313,13 +2316,13 @@
         <v>7</v>
       </c>
       <c r="B84">
-        <v>22317</v>
+        <v>22316</v>
       </c>
       <c r="C84" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D84" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.45">
@@ -2330,10 +2333,10 @@
         <v>22317</v>
       </c>
       <c r="C85" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D85" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.45">
@@ -2344,10 +2347,10 @@
         <v>22317</v>
       </c>
       <c r="C86" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D86" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.45">
@@ -2355,10 +2358,13 @@
         <v>7</v>
       </c>
       <c r="B87">
-        <v>22331</v>
+        <v>22317</v>
+      </c>
+      <c r="C87" t="s">
+        <v>226</v>
       </c>
       <c r="D87" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.45">
@@ -2366,10 +2372,10 @@
         <v>7</v>
       </c>
       <c r="B88">
-        <v>23631</v>
+        <v>22331</v>
       </c>
       <c r="D88" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.45">
@@ -2377,10 +2383,10 @@
         <v>7</v>
       </c>
       <c r="B89">
-        <v>22345</v>
+        <v>23631</v>
       </c>
       <c r="D89" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.45">
@@ -2388,10 +2394,10 @@
         <v>7</v>
       </c>
       <c r="B90">
-        <v>24346</v>
+        <v>22345</v>
       </c>
       <c r="D90" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.45">
@@ -2399,10 +2405,10 @@
         <v>7</v>
       </c>
       <c r="B91">
-        <v>22359</v>
+        <v>24346</v>
       </c>
       <c r="D91" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.45">
@@ -2410,43 +2416,43 @@
         <v>7</v>
       </c>
       <c r="B92">
-        <v>22377</v>
+        <v>22359</v>
       </c>
       <c r="D92" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B93">
-        <v>22356</v>
+        <v>22377</v>
       </c>
       <c r="D93" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B94">
-        <v>22379</v>
+        <v>22356</v>
       </c>
       <c r="D94" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B95">
-        <v>22313</v>
+        <v>22379</v>
       </c>
       <c r="D95" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.45">
@@ -2454,10 +2460,10 @@
         <v>20</v>
       </c>
       <c r="B96">
-        <v>22318</v>
+        <v>22313</v>
       </c>
       <c r="D96" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.45">
@@ -2465,10 +2471,10 @@
         <v>20</v>
       </c>
       <c r="B97">
-        <v>22315</v>
+        <v>22318</v>
       </c>
       <c r="D97" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.45">
@@ -2476,10 +2482,10 @@
         <v>20</v>
       </c>
       <c r="B98">
-        <v>21306</v>
+        <v>22315</v>
       </c>
       <c r="D98" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.45">
@@ -2487,13 +2493,10 @@
         <v>20</v>
       </c>
       <c r="B99">
-        <v>22314</v>
-      </c>
-      <c r="C99" t="s">
-        <v>225</v>
+        <v>21306</v>
       </c>
       <c r="D99" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.45">
@@ -2504,10 +2507,10 @@
         <v>22314</v>
       </c>
       <c r="C100" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D100" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.45">
@@ -2515,10 +2518,13 @@
         <v>20</v>
       </c>
       <c r="B101">
-        <v>22319</v>
+        <v>22314</v>
+      </c>
+      <c r="C101" t="s">
+        <v>226</v>
       </c>
       <c r="D101" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.45">
@@ -2526,10 +2532,10 @@
         <v>20</v>
       </c>
       <c r="B102">
-        <v>22320</v>
+        <v>22319</v>
       </c>
       <c r="D102" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.45">
@@ -2537,10 +2543,10 @@
         <v>20</v>
       </c>
       <c r="B103">
-        <v>21196</v>
+        <v>22320</v>
       </c>
       <c r="D103" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.45">
@@ -2548,24 +2554,21 @@
         <v>20</v>
       </c>
       <c r="B104">
-        <v>21229</v>
+        <v>21196</v>
       </c>
       <c r="D104" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B105">
-        <v>24932</v>
-      </c>
-      <c r="C105" t="s">
-        <v>225</v>
+        <v>21229</v>
       </c>
       <c r="D105" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.45">
@@ -2576,10 +2579,10 @@
         <v>24932</v>
       </c>
       <c r="C106" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D106" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.45">
@@ -2587,24 +2590,24 @@
         <v>16</v>
       </c>
       <c r="B107">
-        <v>24986</v>
+        <v>24932</v>
+      </c>
+      <c r="C107" t="s">
+        <v>226</v>
       </c>
       <c r="D107" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B108">
-        <v>22334</v>
+        <v>24986</v>
       </c>
       <c r="D108" t="s">
-        <v>93</v>
-      </c>
-      <c r="E108" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.45">
@@ -2612,10 +2615,13 @@
         <v>7</v>
       </c>
       <c r="B109">
-        <v>22543</v>
+        <v>22334</v>
       </c>
       <c r="D109" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="E109" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.45">
@@ -2623,10 +2629,10 @@
         <v>7</v>
       </c>
       <c r="B110">
-        <v>23733</v>
+        <v>22543</v>
       </c>
       <c r="D110" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.45">
@@ -2634,10 +2640,10 @@
         <v>7</v>
       </c>
       <c r="B111">
-        <v>22335</v>
+        <v>23733</v>
       </c>
       <c r="D111" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.45">
@@ -2645,10 +2651,10 @@
         <v>7</v>
       </c>
       <c r="B112">
-        <v>22336</v>
+        <v>22335</v>
       </c>
       <c r="D112" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.45">
@@ -2656,10 +2662,10 @@
         <v>7</v>
       </c>
       <c r="B113">
-        <v>23596</v>
+        <v>22336</v>
       </c>
       <c r="D113" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.45">
@@ -2667,10 +2673,10 @@
         <v>7</v>
       </c>
       <c r="B114">
-        <v>22337</v>
+        <v>23596</v>
       </c>
       <c r="D114" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.45">
@@ -2678,10 +2684,10 @@
         <v>7</v>
       </c>
       <c r="B115">
-        <v>22410</v>
+        <v>22337</v>
       </c>
       <c r="D115" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.45">
@@ -2689,10 +2695,10 @@
         <v>7</v>
       </c>
       <c r="B116">
-        <v>22347</v>
+        <v>22410</v>
       </c>
       <c r="D116" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.45">
@@ -2700,10 +2706,10 @@
         <v>7</v>
       </c>
       <c r="B117">
-        <v>22348</v>
+        <v>22347</v>
       </c>
       <c r="D117" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.45">
@@ -2711,10 +2717,10 @@
         <v>7</v>
       </c>
       <c r="B118">
-        <v>22361</v>
+        <v>22348</v>
       </c>
       <c r="D118" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.45">
@@ -2722,10 +2728,10 @@
         <v>7</v>
       </c>
       <c r="B119">
-        <v>22358</v>
+        <v>22361</v>
       </c>
       <c r="D119" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.45">
@@ -2733,10 +2739,10 @@
         <v>7</v>
       </c>
       <c r="B120">
-        <v>22349</v>
+        <v>22358</v>
       </c>
       <c r="D120" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.45">
@@ -2744,10 +2750,10 @@
         <v>7</v>
       </c>
       <c r="B121">
-        <v>22350</v>
+        <v>22349</v>
       </c>
       <c r="D121" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.45">
@@ -2755,10 +2761,10 @@
         <v>7</v>
       </c>
       <c r="B122">
-        <v>22351</v>
+        <v>22350</v>
       </c>
       <c r="D122" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.45">
@@ -2766,10 +2772,10 @@
         <v>7</v>
       </c>
       <c r="B123">
-        <v>22338</v>
+        <v>22351</v>
       </c>
       <c r="D123" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.45">
@@ -2777,10 +2783,10 @@
         <v>7</v>
       </c>
       <c r="B124">
-        <v>22339</v>
+        <v>22338</v>
       </c>
       <c r="D124" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.45">
@@ -2788,10 +2794,10 @@
         <v>7</v>
       </c>
       <c r="B125">
-        <v>22545</v>
+        <v>22339</v>
       </c>
       <c r="D125" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.45">
@@ -2799,10 +2805,10 @@
         <v>7</v>
       </c>
       <c r="B126">
-        <v>23736</v>
+        <v>22545</v>
       </c>
       <c r="D126" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.45">
@@ -2810,10 +2816,10 @@
         <v>7</v>
       </c>
       <c r="B127">
-        <v>22340</v>
+        <v>23736</v>
       </c>
       <c r="D127" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.45">
@@ -2821,10 +2827,10 @@
         <v>7</v>
       </c>
       <c r="B128">
-        <v>22341</v>
+        <v>22340</v>
       </c>
       <c r="D128" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.45">
@@ -2832,10 +2838,10 @@
         <v>7</v>
       </c>
       <c r="B129">
-        <v>23597</v>
+        <v>22341</v>
       </c>
       <c r="D129" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.45">
@@ -2843,21 +2849,21 @@
         <v>7</v>
       </c>
       <c r="B130">
-        <v>22342</v>
+        <v>23597</v>
       </c>
       <c r="D130" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B131">
-        <v>22355</v>
+        <v>22342</v>
       </c>
       <c r="D131" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.45">
@@ -2865,10 +2871,10 @@
         <v>20</v>
       </c>
       <c r="B132">
-        <v>22354</v>
+        <v>22355</v>
       </c>
       <c r="D132" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.45">
@@ -2876,10 +2882,10 @@
         <v>20</v>
       </c>
       <c r="B133">
-        <v>22352</v>
+        <v>22354</v>
       </c>
       <c r="D133" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.45">
@@ -2887,10 +2893,10 @@
         <v>20</v>
       </c>
       <c r="B134">
-        <v>22353</v>
+        <v>22352</v>
       </c>
       <c r="D134" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.45">
@@ -2898,10 +2904,10 @@
         <v>20</v>
       </c>
       <c r="B135">
-        <v>22357</v>
+        <v>22353</v>
       </c>
       <c r="D135" t="s">
-        <v>21</v>
+        <v>119</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.45">
@@ -2909,10 +2915,10 @@
         <v>20</v>
       </c>
       <c r="B136">
-        <v>22411</v>
+        <v>22357</v>
       </c>
       <c r="D136" t="s">
-        <v>120</v>
+        <v>21</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.45">
@@ -2920,10 +2926,10 @@
         <v>20</v>
       </c>
       <c r="B137">
-        <v>24122</v>
+        <v>22411</v>
       </c>
       <c r="D137" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.45">
@@ -2931,21 +2937,21 @@
         <v>20</v>
       </c>
       <c r="B138">
-        <v>25083</v>
+        <v>24122</v>
       </c>
       <c r="D138" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B139">
-        <v>22365</v>
+        <v>25083</v>
       </c>
       <c r="D139" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.45">
@@ -2953,10 +2959,10 @@
         <v>7</v>
       </c>
       <c r="B140">
-        <v>22366</v>
+        <v>22365</v>
       </c>
       <c r="D140" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.45">
@@ -2964,10 +2970,10 @@
         <v>7</v>
       </c>
       <c r="B141">
-        <v>22367</v>
+        <v>22366</v>
       </c>
       <c r="D141" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.45">
@@ -2975,21 +2981,21 @@
         <v>7</v>
       </c>
       <c r="B142">
-        <v>25028</v>
+        <v>22367</v>
       </c>
       <c r="D142" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B143">
-        <v>22584</v>
+        <v>25028</v>
       </c>
       <c r="D143" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.45">
@@ -2997,27 +3003,21 @@
         <v>20</v>
       </c>
       <c r="B144">
-        <v>22547</v>
+        <v>22584</v>
       </c>
       <c r="D144" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B145">
-        <v>22378</v>
-      </c>
-      <c r="C145" t="s">
-        <v>225</v>
+        <v>22547</v>
       </c>
       <c r="D145" t="s">
-        <v>130</v>
-      </c>
-      <c r="E145" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.45">
@@ -3028,10 +3028,13 @@
         <v>22378</v>
       </c>
       <c r="C146" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D146" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="E146" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.45">
@@ -3039,10 +3042,13 @@
         <v>7</v>
       </c>
       <c r="B147">
-        <v>22380</v>
+        <v>22378</v>
+      </c>
+      <c r="C147" t="s">
+        <v>226</v>
       </c>
       <c r="D147" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.45">
@@ -3050,10 +3056,10 @@
         <v>7</v>
       </c>
       <c r="B148">
-        <v>22369</v>
+        <v>22380</v>
       </c>
       <c r="D148" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.45">
@@ -3061,10 +3067,10 @@
         <v>7</v>
       </c>
       <c r="B149">
-        <v>22370</v>
+        <v>22369</v>
       </c>
       <c r="D149" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.45">
@@ -3072,10 +3078,10 @@
         <v>7</v>
       </c>
       <c r="B150">
-        <v>22371</v>
+        <v>22370</v>
       </c>
       <c r="D150" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.45">
@@ -3083,32 +3089,32 @@
         <v>7</v>
       </c>
       <c r="B151">
-        <v>22416</v>
+        <v>22371</v>
       </c>
       <c r="D151" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B152">
-        <v>22548</v>
+        <v>22416</v>
       </c>
       <c r="D152" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B153">
-        <v>22326</v>
+        <v>22548</v>
       </c>
       <c r="D153" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.45">
@@ -3116,10 +3122,10 @@
         <v>7</v>
       </c>
       <c r="B154">
-        <v>22327</v>
+        <v>22326</v>
       </c>
       <c r="D154" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.45">
@@ -3127,10 +3133,10 @@
         <v>7</v>
       </c>
       <c r="B155">
-        <v>22329</v>
+        <v>22327</v>
       </c>
       <c r="D155" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.45">
@@ -3138,10 +3144,10 @@
         <v>7</v>
       </c>
       <c r="B156">
-        <v>22328</v>
+        <v>22329</v>
       </c>
       <c r="D156" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.45">
@@ -3149,10 +3155,10 @@
         <v>7</v>
       </c>
       <c r="B157">
-        <v>22404</v>
+        <v>22328</v>
       </c>
       <c r="D157" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.45">
@@ -3160,10 +3166,10 @@
         <v>7</v>
       </c>
       <c r="B158">
-        <v>22405</v>
+        <v>22404</v>
       </c>
       <c r="D158" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.45">
@@ -3171,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="B159">
-        <v>22406</v>
+        <v>22405</v>
       </c>
       <c r="D159" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.45">
@@ -3182,10 +3188,10 @@
         <v>7</v>
       </c>
       <c r="B160">
-        <v>22419</v>
+        <v>22406</v>
       </c>
       <c r="D160" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.45">
@@ -3193,10 +3199,10 @@
         <v>7</v>
       </c>
       <c r="B161">
-        <v>22407</v>
+        <v>22419</v>
       </c>
       <c r="D161" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.45">
@@ -3204,10 +3210,10 @@
         <v>7</v>
       </c>
       <c r="B162">
-        <v>22408</v>
+        <v>22407</v>
       </c>
       <c r="D162" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.45">
@@ -3215,16 +3221,10 @@
         <v>7</v>
       </c>
       <c r="B163">
-        <v>22309</v>
-      </c>
-      <c r="C163" t="s">
-        <v>225</v>
+        <v>22408</v>
       </c>
       <c r="D163" t="s">
-        <v>149</v>
-      </c>
-      <c r="E163" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.45">
@@ -3235,10 +3235,13 @@
         <v>22309</v>
       </c>
       <c r="C164" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D164" t="s">
-        <v>150</v>
+        <v>149</v>
+      </c>
+      <c r="E164" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.45">
@@ -3246,13 +3249,13 @@
         <v>7</v>
       </c>
       <c r="B165">
-        <v>22310</v>
+        <v>22309</v>
       </c>
       <c r="C165" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D165" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.45">
@@ -3263,10 +3266,10 @@
         <v>22310</v>
       </c>
       <c r="C166" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D166" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.45">
@@ -3274,13 +3277,13 @@
         <v>7</v>
       </c>
       <c r="B167">
-        <v>22311</v>
+        <v>22310</v>
       </c>
       <c r="C167" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D167" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.45">
@@ -3291,10 +3294,10 @@
         <v>22311</v>
       </c>
       <c r="C168" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D168" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.45">
@@ -3302,10 +3305,13 @@
         <v>7</v>
       </c>
       <c r="B169">
-        <v>22312</v>
+        <v>22311</v>
+      </c>
+      <c r="C169" t="s">
+        <v>226</v>
       </c>
       <c r="D169" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.45">
@@ -3313,10 +3319,10 @@
         <v>7</v>
       </c>
       <c r="B170">
-        <v>21274</v>
+        <v>22312</v>
       </c>
       <c r="D170" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.45">
@@ -3324,10 +3330,10 @@
         <v>7</v>
       </c>
       <c r="B171">
-        <v>22414</v>
+        <v>21274</v>
       </c>
       <c r="D171" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.45">
@@ -3335,10 +3341,10 @@
         <v>7</v>
       </c>
       <c r="B172">
-        <v>24044</v>
+        <v>22414</v>
       </c>
       <c r="D172" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.45">
@@ -3346,13 +3352,10 @@
         <v>7</v>
       </c>
       <c r="B173">
-        <v>22312</v>
+        <v>24044</v>
       </c>
       <c r="D173" t="s">
-        <v>155</v>
-      </c>
-      <c r="E173" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.45">
@@ -3360,13 +3363,13 @@
         <v>7</v>
       </c>
       <c r="B174">
-        <v>23179</v>
+        <v>22312</v>
       </c>
       <c r="D174" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E174" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.45">
@@ -3374,10 +3377,13 @@
         <v>7</v>
       </c>
       <c r="B175">
-        <v>23180</v>
+        <v>23179</v>
       </c>
       <c r="D175" t="s">
-        <v>56</v>
+        <v>160</v>
+      </c>
+      <c r="E175" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.45">
@@ -3385,32 +3391,32 @@
         <v>7</v>
       </c>
       <c r="B176">
-        <v>23191</v>
+        <v>23180</v>
       </c>
       <c r="D176" t="s">
-        <v>161</v>
+        <v>56</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B177">
-        <v>15162</v>
+        <v>23191</v>
       </c>
       <c r="D177" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B178">
-        <v>23181</v>
+        <v>15162</v>
       </c>
       <c r="D178" t="s">
-        <v>11</v>
+        <v>162</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.45">
@@ -3418,10 +3424,10 @@
         <v>7</v>
       </c>
       <c r="B179">
-        <v>23182</v>
+        <v>23181</v>
       </c>
       <c r="D179" t="s">
-        <v>93</v>
+        <v>11</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.45">
@@ -3429,10 +3435,10 @@
         <v>7</v>
       </c>
       <c r="B180">
-        <v>23221</v>
+        <v>23182</v>
       </c>
       <c r="D180" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.45">
@@ -3440,10 +3446,10 @@
         <v>7</v>
       </c>
       <c r="B181">
-        <v>23734</v>
+        <v>23221</v>
       </c>
       <c r="D181" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.45">
@@ -3451,10 +3457,10 @@
         <v>7</v>
       </c>
       <c r="B182">
-        <v>23183</v>
+        <v>23734</v>
       </c>
       <c r="D182" t="s">
-        <v>163</v>
+        <v>95</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.45">
@@ -3462,10 +3468,10 @@
         <v>7</v>
       </c>
       <c r="B183">
-        <v>23184</v>
+        <v>23183</v>
       </c>
       <c r="D183" t="s">
-        <v>96</v>
+        <v>163</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.45">
@@ -3473,10 +3479,10 @@
         <v>7</v>
       </c>
       <c r="B184">
-        <v>23185</v>
+        <v>23184</v>
       </c>
       <c r="D184" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.45">
@@ -3484,10 +3490,10 @@
         <v>7</v>
       </c>
       <c r="B185">
-        <v>23210</v>
+        <v>23185</v>
       </c>
       <c r="D185" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.45">
@@ -3495,10 +3501,10 @@
         <v>7</v>
       </c>
       <c r="B186">
-        <v>23186</v>
+        <v>23210</v>
       </c>
       <c r="D186" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.45">
@@ -3506,10 +3512,10 @@
         <v>7</v>
       </c>
       <c r="B187">
-        <v>23187</v>
+        <v>23186</v>
       </c>
       <c r="D187" t="s">
-        <v>164</v>
+        <v>99</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.45">
@@ -3517,10 +3523,10 @@
         <v>7</v>
       </c>
       <c r="B188">
-        <v>23188</v>
+        <v>23187</v>
       </c>
       <c r="D188" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.45">
@@ -3528,10 +3534,10 @@
         <v>7</v>
       </c>
       <c r="B189">
-        <v>23189</v>
+        <v>23188</v>
       </c>
       <c r="D189" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.45">
@@ -3539,10 +3545,10 @@
         <v>7</v>
       </c>
       <c r="B190">
-        <v>23787</v>
+        <v>23189</v>
       </c>
       <c r="D190" t="s">
-        <v>74</v>
+        <v>166</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.45">
@@ -3550,10 +3556,10 @@
         <v>7</v>
       </c>
       <c r="B191">
-        <v>23190</v>
+        <v>23787</v>
       </c>
       <c r="D191" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.45">
@@ -3561,32 +3567,32 @@
         <v>7</v>
       </c>
       <c r="B192">
-        <v>20748</v>
+        <v>23190</v>
       </c>
       <c r="D192" t="s">
-        <v>167</v>
+        <v>57</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B193">
-        <v>24921</v>
+        <v>20748</v>
       </c>
       <c r="D193" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B194">
-        <v>23228</v>
+        <v>24921</v>
       </c>
       <c r="D194" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.45">
@@ -3594,10 +3600,10 @@
         <v>7</v>
       </c>
       <c r="B195">
-        <v>23229</v>
+        <v>23228</v>
       </c>
       <c r="D195" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.45">
@@ -3605,10 +3611,10 @@
         <v>7</v>
       </c>
       <c r="B196">
-        <v>23209</v>
+        <v>23229</v>
       </c>
       <c r="D196" t="s">
-        <v>58</v>
+        <v>170</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.45">
@@ -3616,21 +3622,21 @@
         <v>7</v>
       </c>
       <c r="B197">
-        <v>23206</v>
+        <v>23209</v>
       </c>
       <c r="D197" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B198">
-        <v>25049</v>
+        <v>23206</v>
       </c>
       <c r="D198" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.45">
@@ -3638,10 +3644,10 @@
         <v>20</v>
       </c>
       <c r="B199">
-        <v>26256</v>
+        <v>25049</v>
       </c>
       <c r="D199" t="s">
-        <v>171</v>
+        <v>24</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.45">
@@ -3649,10 +3655,10 @@
         <v>20</v>
       </c>
       <c r="B200">
-        <v>23230</v>
+        <v>26256</v>
       </c>
       <c r="D200" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.45">
@@ -3660,21 +3666,21 @@
         <v>20</v>
       </c>
       <c r="B201">
-        <v>23220</v>
+        <v>23230</v>
       </c>
       <c r="D201" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B202">
-        <v>23196</v>
+        <v>23220</v>
       </c>
       <c r="D202" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.45">
@@ -3682,10 +3688,10 @@
         <v>7</v>
       </c>
       <c r="B203">
-        <v>23194</v>
+        <v>23196</v>
       </c>
       <c r="D203" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.45">
@@ -3693,10 +3699,10 @@
         <v>7</v>
       </c>
       <c r="B204">
-        <v>23195</v>
+        <v>23194</v>
       </c>
       <c r="D204" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.45">
@@ -3704,10 +3710,10 @@
         <v>7</v>
       </c>
       <c r="B205">
-        <v>21770</v>
+        <v>23195</v>
       </c>
       <c r="D205" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.45">
@@ -3715,10 +3721,10 @@
         <v>7</v>
       </c>
       <c r="B206">
-        <v>24824</v>
+        <v>21770</v>
       </c>
       <c r="D206" t="s">
-        <v>64</v>
+        <v>177</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.45">
@@ -3726,10 +3732,10 @@
         <v>7</v>
       </c>
       <c r="B207">
-        <v>24825</v>
+        <v>24824</v>
       </c>
       <c r="D207" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.45">
@@ -3737,10 +3743,10 @@
         <v>7</v>
       </c>
       <c r="B208">
-        <v>23197</v>
+        <v>24825</v>
       </c>
       <c r="D208" t="s">
-        <v>178</v>
+        <v>65</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.45">
@@ -3748,10 +3754,10 @@
         <v>7</v>
       </c>
       <c r="B209">
-        <v>23193</v>
+        <v>23197</v>
       </c>
       <c r="D209" t="s">
-        <v>105</v>
+        <v>178</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.45">
@@ -3759,10 +3765,10 @@
         <v>7</v>
       </c>
       <c r="B210">
-        <v>23192</v>
+        <v>23193</v>
       </c>
       <c r="D210" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.45">
@@ -3770,10 +3776,10 @@
         <v>7</v>
       </c>
       <c r="B211">
-        <v>23198</v>
+        <v>23192</v>
       </c>
       <c r="D211" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.45">
@@ -3781,10 +3787,10 @@
         <v>7</v>
       </c>
       <c r="B212">
-        <v>23207</v>
+        <v>23198</v>
       </c>
       <c r="D212" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.45">
@@ -3792,10 +3798,10 @@
         <v>7</v>
       </c>
       <c r="B213">
-        <v>23208</v>
+        <v>23207</v>
       </c>
       <c r="D213" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.45">
@@ -3803,10 +3809,10 @@
         <v>7</v>
       </c>
       <c r="B214">
-        <v>23232</v>
+        <v>23208</v>
       </c>
       <c r="D214" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.45">
@@ -3814,10 +3820,10 @@
         <v>7</v>
       </c>
       <c r="B215">
-        <v>23204</v>
+        <v>23232</v>
       </c>
       <c r="D215" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.45">
@@ -3825,35 +3831,32 @@
         <v>7</v>
       </c>
       <c r="B216">
-        <v>23205</v>
+        <v>23204</v>
       </c>
       <c r="D216" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A217" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B217">
-        <v>24920</v>
+        <v>23205</v>
       </c>
       <c r="D217" t="s">
-        <v>179</v>
+        <v>28</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A218" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B218">
-        <v>23213</v>
+        <v>24920</v>
       </c>
       <c r="D218" t="s">
-        <v>181</v>
-      </c>
-      <c r="E218" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.45">
@@ -3861,10 +3864,13 @@
         <v>7</v>
       </c>
       <c r="B219">
-        <v>23214</v>
+        <v>23213</v>
       </c>
       <c r="D219" t="s">
-        <v>182</v>
+        <v>181</v>
+      </c>
+      <c r="E219" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.45">
@@ -3872,10 +3878,10 @@
         <v>7</v>
       </c>
       <c r="B220">
-        <v>23215</v>
+        <v>23214</v>
       </c>
       <c r="D220" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.45">
@@ -3883,10 +3889,10 @@
         <v>7</v>
       </c>
       <c r="B221">
-        <v>23216</v>
+        <v>23215</v>
       </c>
       <c r="D221" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.45">
@@ -3894,10 +3900,10 @@
         <v>7</v>
       </c>
       <c r="B222">
-        <v>23218</v>
+        <v>23216</v>
       </c>
       <c r="D222" t="s">
-        <v>96</v>
+        <v>184</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.45">
@@ -3905,10 +3911,10 @@
         <v>7</v>
       </c>
       <c r="B223">
-        <v>23219</v>
+        <v>23218</v>
       </c>
       <c r="D223" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.45">
@@ -3916,10 +3922,10 @@
         <v>7</v>
       </c>
       <c r="B224">
-        <v>26515</v>
+        <v>23219</v>
       </c>
       <c r="D224" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.45">
@@ -3927,10 +3933,10 @@
         <v>7</v>
       </c>
       <c r="B225">
-        <v>23211</v>
+        <v>26515</v>
       </c>
       <c r="D225" t="s">
-        <v>185</v>
+        <v>98</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.45">
@@ -3938,32 +3944,32 @@
         <v>7</v>
       </c>
       <c r="B226">
-        <v>23212</v>
+        <v>23211</v>
       </c>
       <c r="D226" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A227" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B227">
-        <v>23590</v>
+        <v>23212</v>
       </c>
       <c r="D227" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A228" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B228">
-        <v>23231</v>
+        <v>23590</v>
       </c>
       <c r="D228" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.45">
@@ -3971,13 +3977,10 @@
         <v>20</v>
       </c>
       <c r="B229">
-        <v>24974</v>
+        <v>23231</v>
       </c>
       <c r="D229" t="s">
-        <v>190</v>
-      </c>
-      <c r="E229" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.45">
@@ -3985,27 +3988,24 @@
         <v>20</v>
       </c>
       <c r="B230">
-        <v>24990</v>
+        <v>24974</v>
       </c>
       <c r="D230" t="s">
-        <v>191</v>
+        <v>190</v>
+      </c>
+      <c r="E230" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A231" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B231">
-        <v>22423</v>
-      </c>
-      <c r="C231" t="s">
-        <v>241</v>
+        <v>24990</v>
       </c>
       <c r="D231" t="s">
-        <v>55</v>
-      </c>
-      <c r="E231" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.45">
@@ -4016,13 +4016,13 @@
         <v>22423</v>
       </c>
       <c r="C232" t="s">
-        <v>278</v>
+        <v>241</v>
       </c>
       <c r="D232" t="s">
-        <v>280</v>
+        <v>55</v>
       </c>
       <c r="E232" t="s">
-        <v>281</v>
+        <v>192</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.45">
@@ -4030,13 +4030,16 @@
         <v>7</v>
       </c>
       <c r="B233">
-        <v>22487</v>
+        <v>22423</v>
       </c>
       <c r="C233" t="s">
         <v>278</v>
       </c>
       <c r="D233" t="s">
-        <v>283</v>
+        <v>280</v>
+      </c>
+      <c r="E233" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.45">
@@ -4044,13 +4047,13 @@
         <v>7</v>
       </c>
       <c r="B234">
-        <v>22424</v>
+        <v>22487</v>
       </c>
       <c r="C234" t="s">
         <v>278</v>
       </c>
       <c r="D234" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.45">
@@ -4060,8 +4063,11 @@
       <c r="B235">
         <v>22424</v>
       </c>
+      <c r="C235" t="s">
+        <v>278</v>
+      </c>
       <c r="D235" t="s">
-        <v>56</v>
+        <v>282</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.45">
@@ -4069,13 +4075,10 @@
         <v>7</v>
       </c>
       <c r="B236">
-        <v>22444</v>
-      </c>
-      <c r="C236" t="s">
-        <v>241</v>
+        <v>22424</v>
       </c>
       <c r="D236" t="s">
-        <v>161</v>
+        <v>56</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.45">
@@ -4086,10 +4089,10 @@
         <v>22444</v>
       </c>
       <c r="C237" t="s">
-        <v>278</v>
+        <v>241</v>
       </c>
       <c r="D237" t="s">
-        <v>284</v>
+        <v>161</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.45">
@@ -4097,10 +4100,13 @@
         <v>7</v>
       </c>
       <c r="B238">
-        <v>22426</v>
+        <v>22444</v>
+      </c>
+      <c r="C238" t="s">
+        <v>278</v>
       </c>
       <c r="D238" t="s">
-        <v>193</v>
+        <v>284</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.45">
@@ -4108,10 +4114,10 @@
         <v>7</v>
       </c>
       <c r="B239">
-        <v>22542</v>
+        <v>22426</v>
       </c>
       <c r="D239" t="s">
-        <v>94</v>
+        <v>193</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.45">
@@ -4119,10 +4125,10 @@
         <v>7</v>
       </c>
       <c r="B240">
-        <v>23732</v>
+        <v>22542</v>
       </c>
       <c r="D240" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.45">
@@ -4130,10 +4136,10 @@
         <v>7</v>
       </c>
       <c r="B241">
-        <v>22427</v>
+        <v>23732</v>
       </c>
       <c r="D241" t="s">
-        <v>163</v>
+        <v>95</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.45">
@@ -4141,10 +4147,10 @@
         <v>7</v>
       </c>
       <c r="B242">
-        <v>22428</v>
+        <v>22427</v>
       </c>
       <c r="D242" t="s">
-        <v>96</v>
+        <v>163</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.45">
@@ -4152,10 +4158,10 @@
         <v>7</v>
       </c>
       <c r="B243">
-        <v>22429</v>
+        <v>22428</v>
       </c>
       <c r="D243" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.45">
@@ -4163,10 +4169,10 @@
         <v>7</v>
       </c>
       <c r="B244">
-        <v>23600</v>
+        <v>22429</v>
       </c>
       <c r="D244" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.45">
@@ -4174,10 +4180,10 @@
         <v>7</v>
       </c>
       <c r="B245">
-        <v>22430</v>
+        <v>23600</v>
       </c>
       <c r="D245" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.45">
@@ -4185,10 +4191,10 @@
         <v>7</v>
       </c>
       <c r="B246">
-        <v>22483</v>
+        <v>22430</v>
       </c>
       <c r="D246" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.45">
@@ -4196,10 +4202,10 @@
         <v>7</v>
       </c>
       <c r="B247">
-        <v>22431</v>
+        <v>22483</v>
       </c>
       <c r="D247" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.45">
@@ -4207,10 +4213,10 @@
         <v>7</v>
       </c>
       <c r="B248">
-        <v>22432</v>
+        <v>22431</v>
       </c>
       <c r="D248" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.45">
@@ -4218,10 +4224,10 @@
         <v>7</v>
       </c>
       <c r="B249">
-        <v>23628</v>
+        <v>22432</v>
       </c>
       <c r="D249" t="s">
-        <v>194</v>
+        <v>165</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.45">
@@ -4229,10 +4235,10 @@
         <v>7</v>
       </c>
       <c r="B250">
-        <v>22433</v>
+        <v>23628</v>
       </c>
       <c r="D250" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.45">
@@ -4240,10 +4246,10 @@
         <v>7</v>
       </c>
       <c r="B251">
-        <v>22425</v>
+        <v>22433</v>
       </c>
       <c r="D251" t="s">
-        <v>11</v>
+        <v>166</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.45">
@@ -4251,10 +4257,10 @@
         <v>7</v>
       </c>
       <c r="B252">
-        <v>23808</v>
+        <v>22425</v>
       </c>
       <c r="D252" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.45">
@@ -4262,10 +4268,10 @@
         <v>7</v>
       </c>
       <c r="B253">
-        <v>22443</v>
+        <v>23808</v>
       </c>
       <c r="D253" t="s">
-        <v>195</v>
+        <v>74</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.45">
@@ -4273,10 +4279,10 @@
         <v>7</v>
       </c>
       <c r="B254">
-        <v>20747</v>
+        <v>22443</v>
       </c>
       <c r="D254" t="s">
-        <v>167</v>
+        <v>195</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.45">
@@ -4284,10 +4290,10 @@
         <v>7</v>
       </c>
       <c r="B255">
-        <v>22485</v>
+        <v>20747</v>
       </c>
       <c r="D255" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.45">
@@ -4295,10 +4301,10 @@
         <v>7</v>
       </c>
       <c r="B256">
-        <v>22434</v>
+        <v>22485</v>
       </c>
       <c r="D256" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.45">
@@ -4306,10 +4312,10 @@
         <v>7</v>
       </c>
       <c r="B257">
-        <v>22435</v>
+        <v>22434</v>
       </c>
       <c r="D257" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.45">
@@ -4317,10 +4323,10 @@
         <v>7</v>
       </c>
       <c r="B258">
-        <v>22544</v>
+        <v>22435</v>
       </c>
       <c r="D258" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.45">
@@ -4328,10 +4334,10 @@
         <v>7</v>
       </c>
       <c r="B259">
-        <v>23735</v>
+        <v>22544</v>
       </c>
       <c r="D259" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.45">
@@ -4339,10 +4345,10 @@
         <v>7</v>
       </c>
       <c r="B260">
-        <v>22436</v>
+        <v>23735</v>
       </c>
       <c r="D260" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.45">
@@ -4350,10 +4356,10 @@
         <v>7</v>
       </c>
       <c r="B261">
-        <v>22437</v>
+        <v>22436</v>
       </c>
       <c r="D261" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.45">
@@ -4361,10 +4367,10 @@
         <v>7</v>
       </c>
       <c r="B262">
-        <v>22438</v>
+        <v>22437</v>
       </c>
       <c r="D262" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.45">
@@ -4372,10 +4378,10 @@
         <v>7</v>
       </c>
       <c r="B263">
-        <v>23601</v>
+        <v>22438</v>
       </c>
       <c r="D263" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.45">
@@ -4383,10 +4389,10 @@
         <v>7</v>
       </c>
       <c r="B264">
-        <v>22439</v>
+        <v>23601</v>
       </c>
       <c r="D264" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.45">
@@ -4394,10 +4400,10 @@
         <v>7</v>
       </c>
       <c r="B265">
-        <v>22440</v>
+        <v>22439</v>
       </c>
       <c r="D265" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.45">
@@ -4405,10 +4411,10 @@
         <v>7</v>
       </c>
       <c r="B266">
-        <v>22441</v>
+        <v>22440</v>
       </c>
       <c r="D266" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.45">
@@ -4416,10 +4422,10 @@
         <v>7</v>
       </c>
       <c r="B267">
-        <v>23626</v>
+        <v>22441</v>
       </c>
       <c r="D267" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.45">
@@ -4427,10 +4433,10 @@
         <v>7</v>
       </c>
       <c r="B268">
-        <v>22442</v>
+        <v>23626</v>
       </c>
       <c r="D268" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.45">
@@ -4438,13 +4444,10 @@
         <v>7</v>
       </c>
       <c r="B269">
-        <v>22446</v>
-      </c>
-      <c r="C269" t="s">
-        <v>241</v>
+        <v>22442</v>
       </c>
       <c r="D269" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.45">
@@ -4455,10 +4458,10 @@
         <v>22446</v>
       </c>
       <c r="C270" t="s">
-        <v>278</v>
+        <v>241</v>
       </c>
       <c r="D270" t="s">
-        <v>285</v>
+        <v>209</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.45">
@@ -4466,13 +4469,13 @@
         <v>7</v>
       </c>
       <c r="B271">
-        <v>22587</v>
+        <v>22446</v>
       </c>
       <c r="C271" t="s">
         <v>278</v>
       </c>
       <c r="D271" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.45">
@@ -4480,13 +4483,13 @@
         <v>7</v>
       </c>
       <c r="B272">
-        <v>22588</v>
+        <v>22587</v>
       </c>
       <c r="C272" t="s">
         <v>278</v>
       </c>
       <c r="D272" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.45">
@@ -4494,13 +4497,13 @@
         <v>7</v>
       </c>
       <c r="B273">
-        <v>22589</v>
+        <v>22588</v>
       </c>
       <c r="C273" t="s">
         <v>278</v>
       </c>
       <c r="D273" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.45">
@@ -4508,13 +4511,13 @@
         <v>7</v>
       </c>
       <c r="B274">
-        <v>22590</v>
+        <v>22589</v>
       </c>
       <c r="C274" t="s">
         <v>278</v>
       </c>
       <c r="D274" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.45">
@@ -4522,13 +4525,13 @@
         <v>7</v>
       </c>
       <c r="B275">
-        <v>22591</v>
+        <v>22590</v>
       </c>
       <c r="C275" t="s">
         <v>278</v>
       </c>
       <c r="D275" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.45">
@@ -4536,13 +4539,13 @@
         <v>7</v>
       </c>
       <c r="B276">
-        <v>22592</v>
+        <v>22591</v>
       </c>
       <c r="C276" t="s">
         <v>278</v>
       </c>
       <c r="D276" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.45">
@@ -4550,13 +4553,13 @@
         <v>7</v>
       </c>
       <c r="B277">
-        <v>22593</v>
+        <v>22592</v>
       </c>
       <c r="C277" t="s">
         <v>278</v>
       </c>
       <c r="D277" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.45">
@@ -4564,13 +4567,13 @@
         <v>7</v>
       </c>
       <c r="B278">
-        <v>22594</v>
+        <v>22593</v>
       </c>
       <c r="C278" t="s">
         <v>278</v>
       </c>
       <c r="D278" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.45">
@@ -4578,13 +4581,13 @@
         <v>7</v>
       </c>
       <c r="B279">
-        <v>22595</v>
+        <v>22594</v>
       </c>
       <c r="C279" t="s">
         <v>278</v>
       </c>
       <c r="D279" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.45">
@@ -4592,38 +4595,41 @@
         <v>7</v>
       </c>
       <c r="B280">
-        <v>22596</v>
+        <v>22595</v>
       </c>
       <c r="C280" t="s">
         <v>278</v>
       </c>
       <c r="D280" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A281" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B281">
-        <v>26572</v>
+        <v>22596</v>
       </c>
       <c r="C281" t="s">
         <v>278</v>
       </c>
       <c r="D281" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A282" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B282">
-        <v>22447</v>
+        <v>26572</v>
+      </c>
+      <c r="C282" t="s">
+        <v>278</v>
       </c>
       <c r="D282" t="s">
-        <v>101</v>
+        <v>296</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.45">
@@ -4631,10 +4637,10 @@
         <v>7</v>
       </c>
       <c r="B283">
-        <v>22448</v>
+        <v>22447</v>
       </c>
       <c r="D283" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.45">
@@ -4642,13 +4648,10 @@
         <v>7</v>
       </c>
       <c r="B284">
-        <v>22450</v>
+        <v>22448</v>
       </c>
       <c r="D284" t="s">
-        <v>60</v>
-      </c>
-      <c r="E284" t="s">
-        <v>210</v>
+        <v>102</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.45">
@@ -4656,10 +4659,13 @@
         <v>7</v>
       </c>
       <c r="B285">
-        <v>22449</v>
+        <v>22450</v>
       </c>
       <c r="D285" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="E285" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.45">
@@ -4667,10 +4673,10 @@
         <v>7</v>
       </c>
       <c r="B286">
-        <v>22451</v>
+        <v>22449</v>
       </c>
       <c r="D286" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.45">
@@ -4678,10 +4684,10 @@
         <v>7</v>
       </c>
       <c r="B287">
-        <v>23737</v>
+        <v>22451</v>
       </c>
       <c r="D287" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.45">
@@ -4689,10 +4695,10 @@
         <v>7</v>
       </c>
       <c r="B288">
-        <v>22457</v>
+        <v>23737</v>
       </c>
       <c r="D288" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.45">
@@ -4700,10 +4706,10 @@
         <v>7</v>
       </c>
       <c r="B289">
-        <v>22456</v>
+        <v>22457</v>
       </c>
       <c r="D289" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.45">
@@ -4711,10 +4717,10 @@
         <v>7</v>
       </c>
       <c r="B290">
-        <v>24821</v>
+        <v>22456</v>
       </c>
       <c r="D290" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.45">
@@ -4722,10 +4728,10 @@
         <v>7</v>
       </c>
       <c r="B291">
-        <v>24822</v>
+        <v>24821</v>
       </c>
       <c r="D291" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.45">
@@ -4733,10 +4739,10 @@
         <v>7</v>
       </c>
       <c r="B292">
-        <v>22481</v>
+        <v>24822</v>
       </c>
       <c r="D292" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.45">
@@ -4744,10 +4750,10 @@
         <v>7</v>
       </c>
       <c r="B293">
-        <v>22479</v>
+        <v>22481</v>
       </c>
       <c r="D293" t="s">
-        <v>175</v>
+        <v>18</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.45">
@@ -4755,10 +4761,10 @@
         <v>7</v>
       </c>
       <c r="B294">
-        <v>22480</v>
+        <v>22479</v>
       </c>
       <c r="D294" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.45">
@@ -4766,10 +4772,10 @@
         <v>7</v>
       </c>
       <c r="B295">
-        <v>22467</v>
+        <v>22480</v>
       </c>
       <c r="D295" t="s">
-        <v>211</v>
+        <v>176</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.45">
@@ -4777,10 +4783,10 @@
         <v>7</v>
       </c>
       <c r="B296">
-        <v>22458</v>
+        <v>22467</v>
       </c>
       <c r="D296" t="s">
-        <v>103</v>
+        <v>211</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.45">
@@ -4788,10 +4794,10 @@
         <v>7</v>
       </c>
       <c r="B297">
-        <v>22462</v>
+        <v>22458</v>
       </c>
       <c r="D297" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.45">
@@ -4799,10 +4805,10 @@
         <v>7</v>
       </c>
       <c r="B298">
-        <v>22463</v>
+        <v>22462</v>
       </c>
       <c r="D298" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.45">
@@ -4810,10 +4816,10 @@
         <v>7</v>
       </c>
       <c r="B299">
-        <v>22464</v>
+        <v>22463</v>
       </c>
       <c r="D299" t="s">
-        <v>269</v>
+        <v>75</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.45">
@@ -4821,10 +4827,10 @@
         <v>7</v>
       </c>
       <c r="B300">
-        <v>22486</v>
+        <v>22464</v>
       </c>
       <c r="D300" t="s">
-        <v>26</v>
+        <v>269</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.45">
@@ -4832,10 +4838,10 @@
         <v>7</v>
       </c>
       <c r="B301">
-        <v>22465</v>
+        <v>22486</v>
       </c>
       <c r="D301" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.45">
@@ -4843,10 +4849,10 @@
         <v>7</v>
       </c>
       <c r="B302">
-        <v>22466</v>
+        <v>22465</v>
       </c>
       <c r="D302" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.45">
@@ -4854,10 +4860,10 @@
         <v>7</v>
       </c>
       <c r="B303">
-        <v>26461</v>
+        <v>22466</v>
       </c>
       <c r="D303" t="s">
-        <v>212</v>
+        <v>28</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.45">
@@ -4865,24 +4871,21 @@
         <v>7</v>
       </c>
       <c r="B304">
-        <v>26462</v>
+        <v>26461</v>
       </c>
       <c r="D304" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A305" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B305">
-        <v>24838</v>
+        <v>26462</v>
       </c>
       <c r="D305" t="s">
-        <v>215</v>
-      </c>
-      <c r="E305" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.45">
@@ -4890,10 +4893,13 @@
         <v>16</v>
       </c>
       <c r="B306">
-        <v>24842</v>
+        <v>24838</v>
       </c>
       <c r="D306" t="s">
-        <v>216</v>
+        <v>215</v>
+      </c>
+      <c r="E306" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.45">
@@ -4901,10 +4907,10 @@
         <v>16</v>
       </c>
       <c r="B307">
-        <v>24846</v>
+        <v>24842</v>
       </c>
       <c r="D307" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.45">
@@ -4912,10 +4918,10 @@
         <v>16</v>
       </c>
       <c r="B308">
-        <v>24849</v>
+        <v>24846</v>
       </c>
       <c r="D308" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.45">
@@ -4923,10 +4929,10 @@
         <v>16</v>
       </c>
       <c r="B309">
-        <v>24852</v>
+        <v>24849</v>
       </c>
       <c r="D309" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.45">
@@ -4934,10 +4940,10 @@
         <v>16</v>
       </c>
       <c r="B310">
-        <v>24856</v>
+        <v>24852</v>
       </c>
       <c r="D310" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.45">
@@ -4945,24 +4951,21 @@
         <v>16</v>
       </c>
       <c r="B311">
-        <v>24859</v>
+        <v>24856</v>
       </c>
       <c r="D311" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A312" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B312">
-        <v>7315</v>
+        <v>24859</v>
       </c>
       <c r="D312" t="s">
-        <v>223</v>
-      </c>
-      <c r="E312" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.45">
@@ -4970,21 +4973,24 @@
         <v>20</v>
       </c>
       <c r="B313">
-        <v>7316</v>
+        <v>7315</v>
       </c>
       <c r="D313" t="s">
-        <v>224</v>
+        <v>223</v>
+      </c>
+      <c r="E313" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A314" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B314">
-        <v>6818</v>
+        <v>7316</v>
       </c>
       <c r="D314" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.45">
@@ -4992,13 +4998,10 @@
         <v>7</v>
       </c>
       <c r="B315">
-        <v>23566</v>
+        <v>6818</v>
       </c>
       <c r="D315" t="s">
-        <v>231</v>
-      </c>
-      <c r="E315" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.45">
@@ -5006,10 +5009,13 @@
         <v>7</v>
       </c>
       <c r="B316">
-        <v>23567</v>
+        <v>23566</v>
       </c>
       <c r="D316" t="s">
-        <v>56</v>
+        <v>231</v>
+      </c>
+      <c r="E316" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.45">
@@ -5017,10 +5023,10 @@
         <v>7</v>
       </c>
       <c r="B317">
-        <v>24655</v>
+        <v>23567</v>
       </c>
       <c r="D317" t="s">
-        <v>232</v>
+        <v>56</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.45">
@@ -5028,13 +5034,10 @@
         <v>7</v>
       </c>
       <c r="B318">
-        <v>23233</v>
+        <v>24655</v>
       </c>
       <c r="D318" t="s">
-        <v>271</v>
-      </c>
-      <c r="E318" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.45">
@@ -5042,10 +5045,13 @@
         <v>7</v>
       </c>
       <c r="B319">
-        <v>23234</v>
+        <v>23233</v>
       </c>
       <c r="D319" t="s">
-        <v>160</v>
+        <v>271</v>
+      </c>
+      <c r="E319" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.45">
@@ -5053,10 +5059,10 @@
         <v>7</v>
       </c>
       <c r="B320">
-        <v>23235</v>
+        <v>23234</v>
       </c>
       <c r="D320" t="s">
-        <v>56</v>
+        <v>160</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.45">
@@ -5064,10 +5070,10 @@
         <v>7</v>
       </c>
       <c r="B321">
-        <v>23240</v>
+        <v>23235</v>
       </c>
       <c r="D321" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.45">
@@ -5075,10 +5081,10 @@
         <v>7</v>
       </c>
       <c r="B322">
-        <v>23239</v>
+        <v>23240</v>
       </c>
       <c r="D322" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.45">
@@ -5086,10 +5092,10 @@
         <v>7</v>
       </c>
       <c r="B323">
-        <v>23237</v>
+        <v>23239</v>
       </c>
       <c r="D323" t="s">
-        <v>272</v>
+        <v>54</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.45">
@@ -5097,10 +5103,10 @@
         <v>7</v>
       </c>
       <c r="B324">
-        <v>23257</v>
+        <v>23237</v>
       </c>
       <c r="D324" t="s">
-        <v>177</v>
+        <v>272</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.45">
@@ -5108,10 +5114,10 @@
         <v>7</v>
       </c>
       <c r="B325">
-        <v>23251</v>
+        <v>23257</v>
       </c>
       <c r="D325" t="s">
-        <v>273</v>
+        <v>177</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.45">
@@ -5119,10 +5125,10 @@
         <v>7</v>
       </c>
       <c r="B326">
-        <v>23241</v>
+        <v>23251</v>
       </c>
       <c r="D326" t="s">
-        <v>68</v>
+        <v>273</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.45">
@@ -5130,10 +5136,10 @@
         <v>7</v>
       </c>
       <c r="B327">
-        <v>23242</v>
+        <v>23241</v>
       </c>
       <c r="D327" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.45">
@@ -5141,10 +5147,10 @@
         <v>7</v>
       </c>
       <c r="B328">
-        <v>23255</v>
+        <v>23242</v>
       </c>
       <c r="D328" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.45">
@@ -5152,10 +5158,10 @@
         <v>7</v>
       </c>
       <c r="B329">
-        <v>23254</v>
+        <v>23255</v>
       </c>
       <c r="D329" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.45">
@@ -5163,10 +5169,10 @@
         <v>7</v>
       </c>
       <c r="B330">
-        <v>23243</v>
+        <v>23254</v>
       </c>
       <c r="D330" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.45">
@@ -5174,10 +5180,32 @@
         <v>7</v>
       </c>
       <c r="B331">
+        <v>23243</v>
+      </c>
+      <c r="D331" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A332" t="s">
+        <v>7</v>
+      </c>
+      <c r="B332">
         <v>23244</v>
       </c>
-      <c r="D331" t="s">
+      <c r="D332" t="s">
         <v>274</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A333" t="s">
+        <v>16</v>
+      </c>
+      <c r="B333">
+        <v>25019</v>
+      </c>
+      <c r="D333" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a missing label for customer.
</commit_message>
<xml_diff>
--- a/Controls.xlsx
+++ b/Controls.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl-Otto\Documents\src\NVDA\vismaadministration-nvdaaddon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2553B51-9FB9-4109-8C90-BFBAB8DE9B75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD5DCDA-92C2-436C-B12D-979F2E126C4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="735" yWindow="735" windowWidth="23040" windowHeight="12232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="303">
   <si>
     <t>WindowClassName</t>
   </si>
@@ -961,6 +961,9 @@
   </si>
   <si>
     <t>Inställningar för egen kopia, utskriftsval</t>
+  </si>
+  <si>
+    <t>Kundfordranskonto</t>
   </si>
 </sst>
 </file>
@@ -1278,10 +1281,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E333"/>
+  <dimension ref="A1:E334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A306" workbookViewId="0">
-      <selection activeCell="D333" sqref="D333"/>
+    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
+      <selection activeCell="D212" sqref="D212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3787,10 +3790,10 @@
         <v>7</v>
       </c>
       <c r="B212">
-        <v>23198</v>
+        <v>26598</v>
       </c>
       <c r="D212" t="s">
-        <v>60</v>
+        <v>302</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.45">
@@ -3798,10 +3801,10 @@
         <v>7</v>
       </c>
       <c r="B213">
-        <v>23207</v>
+        <v>23198</v>
       </c>
       <c r="D213" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.45">
@@ -3809,10 +3812,10 @@
         <v>7</v>
       </c>
       <c r="B214">
-        <v>23208</v>
+        <v>23207</v>
       </c>
       <c r="D214" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.45">
@@ -3820,10 +3823,10 @@
         <v>7</v>
       </c>
       <c r="B215">
-        <v>23232</v>
+        <v>23208</v>
       </c>
       <c r="D215" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.45">
@@ -3831,10 +3834,10 @@
         <v>7</v>
       </c>
       <c r="B216">
-        <v>23204</v>
+        <v>23232</v>
       </c>
       <c r="D216" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.45">
@@ -3842,35 +3845,32 @@
         <v>7</v>
       </c>
       <c r="B217">
-        <v>23205</v>
+        <v>23204</v>
       </c>
       <c r="D217" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A218" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B218">
-        <v>24920</v>
+        <v>23205</v>
       </c>
       <c r="D218" t="s">
-        <v>179</v>
+        <v>28</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A219" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B219">
-        <v>23213</v>
+        <v>24920</v>
       </c>
       <c r="D219" t="s">
-        <v>181</v>
-      </c>
-      <c r="E219" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.45">
@@ -3878,10 +3878,13 @@
         <v>7</v>
       </c>
       <c r="B220">
-        <v>23214</v>
+        <v>23213</v>
       </c>
       <c r="D220" t="s">
-        <v>182</v>
+        <v>181</v>
+      </c>
+      <c r="E220" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.45">
@@ -3889,10 +3892,10 @@
         <v>7</v>
       </c>
       <c r="B221">
-        <v>23215</v>
+        <v>23214</v>
       </c>
       <c r="D221" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.45">
@@ -3900,10 +3903,10 @@
         <v>7</v>
       </c>
       <c r="B222">
-        <v>23216</v>
+        <v>23215</v>
       </c>
       <c r="D222" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.45">
@@ -3911,10 +3914,10 @@
         <v>7</v>
       </c>
       <c r="B223">
-        <v>23218</v>
+        <v>23216</v>
       </c>
       <c r="D223" t="s">
-        <v>96</v>
+        <v>184</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.45">
@@ -3922,10 +3925,10 @@
         <v>7</v>
       </c>
       <c r="B224">
-        <v>23219</v>
+        <v>23218</v>
       </c>
       <c r="D224" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.45">
@@ -3933,10 +3936,10 @@
         <v>7</v>
       </c>
       <c r="B225">
-        <v>26515</v>
+        <v>23219</v>
       </c>
       <c r="D225" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.45">
@@ -3944,10 +3947,10 @@
         <v>7</v>
       </c>
       <c r="B226">
-        <v>23211</v>
+        <v>26515</v>
       </c>
       <c r="D226" t="s">
-        <v>185</v>
+        <v>98</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.45">
@@ -3955,32 +3958,32 @@
         <v>7</v>
       </c>
       <c r="B227">
-        <v>23212</v>
+        <v>23211</v>
       </c>
       <c r="D227" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A228" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B228">
-        <v>23590</v>
+        <v>23212</v>
       </c>
       <c r="D228" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A229" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B229">
-        <v>23231</v>
+        <v>23590</v>
       </c>
       <c r="D229" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.45">
@@ -3988,13 +3991,10 @@
         <v>20</v>
       </c>
       <c r="B230">
-        <v>24974</v>
+        <v>23231</v>
       </c>
       <c r="D230" t="s">
-        <v>190</v>
-      </c>
-      <c r="E230" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.45">
@@ -4002,27 +4002,24 @@
         <v>20</v>
       </c>
       <c r="B231">
-        <v>24990</v>
+        <v>24974</v>
       </c>
       <c r="D231" t="s">
-        <v>191</v>
+        <v>190</v>
+      </c>
+      <c r="E231" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A232" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B232">
-        <v>22423</v>
-      </c>
-      <c r="C232" t="s">
-        <v>241</v>
+        <v>24990</v>
       </c>
       <c r="D232" t="s">
-        <v>55</v>
-      </c>
-      <c r="E232" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.45">
@@ -4033,13 +4030,13 @@
         <v>22423</v>
       </c>
       <c r="C233" t="s">
-        <v>278</v>
+        <v>241</v>
       </c>
       <c r="D233" t="s">
-        <v>280</v>
+        <v>55</v>
       </c>
       <c r="E233" t="s">
-        <v>281</v>
+        <v>192</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.45">
@@ -4047,13 +4044,16 @@
         <v>7</v>
       </c>
       <c r="B234">
-        <v>22487</v>
+        <v>22423</v>
       </c>
       <c r="C234" t="s">
         <v>278</v>
       </c>
       <c r="D234" t="s">
-        <v>283</v>
+        <v>280</v>
+      </c>
+      <c r="E234" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.45">
@@ -4061,13 +4061,13 @@
         <v>7</v>
       </c>
       <c r="B235">
-        <v>22424</v>
+        <v>22487</v>
       </c>
       <c r="C235" t="s">
         <v>278</v>
       </c>
       <c r="D235" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.45">
@@ -4077,8 +4077,11 @@
       <c r="B236">
         <v>22424</v>
       </c>
+      <c r="C236" t="s">
+        <v>278</v>
+      </c>
       <c r="D236" t="s">
-        <v>56</v>
+        <v>282</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.45">
@@ -4086,13 +4089,10 @@
         <v>7</v>
       </c>
       <c r="B237">
-        <v>22444</v>
-      </c>
-      <c r="C237" t="s">
-        <v>241</v>
+        <v>22424</v>
       </c>
       <c r="D237" t="s">
-        <v>161</v>
+        <v>56</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.45">
@@ -4103,10 +4103,10 @@
         <v>22444</v>
       </c>
       <c r="C238" t="s">
-        <v>278</v>
+        <v>241</v>
       </c>
       <c r="D238" t="s">
-        <v>284</v>
+        <v>161</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.45">
@@ -4114,10 +4114,13 @@
         <v>7</v>
       </c>
       <c r="B239">
-        <v>22426</v>
+        <v>22444</v>
+      </c>
+      <c r="C239" t="s">
+        <v>278</v>
       </c>
       <c r="D239" t="s">
-        <v>193</v>
+        <v>284</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.45">
@@ -4125,10 +4128,10 @@
         <v>7</v>
       </c>
       <c r="B240">
-        <v>22542</v>
+        <v>22426</v>
       </c>
       <c r="D240" t="s">
-        <v>94</v>
+        <v>193</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.45">
@@ -4136,10 +4139,10 @@
         <v>7</v>
       </c>
       <c r="B241">
-        <v>23732</v>
+        <v>22542</v>
       </c>
       <c r="D241" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.45">
@@ -4147,10 +4150,10 @@
         <v>7</v>
       </c>
       <c r="B242">
-        <v>22427</v>
+        <v>23732</v>
       </c>
       <c r="D242" t="s">
-        <v>163</v>
+        <v>95</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.45">
@@ -4158,10 +4161,10 @@
         <v>7</v>
       </c>
       <c r="B243">
-        <v>22428</v>
+        <v>22427</v>
       </c>
       <c r="D243" t="s">
-        <v>96</v>
+        <v>163</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.45">
@@ -4169,10 +4172,10 @@
         <v>7</v>
       </c>
       <c r="B244">
-        <v>22429</v>
+        <v>22428</v>
       </c>
       <c r="D244" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.45">
@@ -4180,10 +4183,10 @@
         <v>7</v>
       </c>
       <c r="B245">
-        <v>23600</v>
+        <v>22429</v>
       </c>
       <c r="D245" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.45">
@@ -4191,10 +4194,10 @@
         <v>7</v>
       </c>
       <c r="B246">
-        <v>22430</v>
+        <v>23600</v>
       </c>
       <c r="D246" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.45">
@@ -4202,10 +4205,10 @@
         <v>7</v>
       </c>
       <c r="B247">
-        <v>22483</v>
+        <v>22430</v>
       </c>
       <c r="D247" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.45">
@@ -4213,10 +4216,10 @@
         <v>7</v>
       </c>
       <c r="B248">
-        <v>22431</v>
+        <v>22483</v>
       </c>
       <c r="D248" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.45">
@@ -4224,10 +4227,10 @@
         <v>7</v>
       </c>
       <c r="B249">
-        <v>22432</v>
+        <v>22431</v>
       </c>
       <c r="D249" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.45">
@@ -4235,10 +4238,10 @@
         <v>7</v>
       </c>
       <c r="B250">
-        <v>23628</v>
+        <v>22432</v>
       </c>
       <c r="D250" t="s">
-        <v>194</v>
+        <v>165</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.45">
@@ -4246,10 +4249,10 @@
         <v>7</v>
       </c>
       <c r="B251">
-        <v>22433</v>
+        <v>23628</v>
       </c>
       <c r="D251" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.45">
@@ -4257,10 +4260,10 @@
         <v>7</v>
       </c>
       <c r="B252">
-        <v>22425</v>
+        <v>22433</v>
       </c>
       <c r="D252" t="s">
-        <v>11</v>
+        <v>166</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.45">
@@ -4268,10 +4271,10 @@
         <v>7</v>
       </c>
       <c r="B253">
-        <v>23808</v>
+        <v>22425</v>
       </c>
       <c r="D253" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.45">
@@ -4279,10 +4282,10 @@
         <v>7</v>
       </c>
       <c r="B254">
-        <v>22443</v>
+        <v>23808</v>
       </c>
       <c r="D254" t="s">
-        <v>195</v>
+        <v>74</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.45">
@@ -4290,10 +4293,10 @@
         <v>7</v>
       </c>
       <c r="B255">
-        <v>20747</v>
+        <v>22443</v>
       </c>
       <c r="D255" t="s">
-        <v>167</v>
+        <v>195</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.45">
@@ -4301,10 +4304,10 @@
         <v>7</v>
       </c>
       <c r="B256">
-        <v>22485</v>
+        <v>20747</v>
       </c>
       <c r="D256" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.45">
@@ -4312,10 +4315,10 @@
         <v>7</v>
       </c>
       <c r="B257">
-        <v>22434</v>
+        <v>22485</v>
       </c>
       <c r="D257" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.45">
@@ -4323,10 +4326,10 @@
         <v>7</v>
       </c>
       <c r="B258">
-        <v>22435</v>
+        <v>22434</v>
       </c>
       <c r="D258" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.45">
@@ -4334,10 +4337,10 @@
         <v>7</v>
       </c>
       <c r="B259">
-        <v>22544</v>
+        <v>22435</v>
       </c>
       <c r="D259" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.45">
@@ -4345,10 +4348,10 @@
         <v>7</v>
       </c>
       <c r="B260">
-        <v>23735</v>
+        <v>22544</v>
       </c>
       <c r="D260" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.45">
@@ -4356,10 +4359,10 @@
         <v>7</v>
       </c>
       <c r="B261">
-        <v>22436</v>
+        <v>23735</v>
       </c>
       <c r="D261" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.45">
@@ -4367,10 +4370,10 @@
         <v>7</v>
       </c>
       <c r="B262">
-        <v>22437</v>
+        <v>22436</v>
       </c>
       <c r="D262" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.45">
@@ -4378,10 +4381,10 @@
         <v>7</v>
       </c>
       <c r="B263">
-        <v>22438</v>
+        <v>22437</v>
       </c>
       <c r="D263" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.45">
@@ -4389,10 +4392,10 @@
         <v>7</v>
       </c>
       <c r="B264">
-        <v>23601</v>
+        <v>22438</v>
       </c>
       <c r="D264" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.45">
@@ -4400,10 +4403,10 @@
         <v>7</v>
       </c>
       <c r="B265">
-        <v>22439</v>
+        <v>23601</v>
       </c>
       <c r="D265" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.45">
@@ -4411,10 +4414,10 @@
         <v>7</v>
       </c>
       <c r="B266">
-        <v>22440</v>
+        <v>22439</v>
       </c>
       <c r="D266" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.45">
@@ -4422,10 +4425,10 @@
         <v>7</v>
       </c>
       <c r="B267">
-        <v>22441</v>
+        <v>22440</v>
       </c>
       <c r="D267" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.45">
@@ -4433,10 +4436,10 @@
         <v>7</v>
       </c>
       <c r="B268">
-        <v>23626</v>
+        <v>22441</v>
       </c>
       <c r="D268" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.45">
@@ -4444,10 +4447,10 @@
         <v>7</v>
       </c>
       <c r="B269">
-        <v>22442</v>
+        <v>23626</v>
       </c>
       <c r="D269" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.45">
@@ -4455,13 +4458,10 @@
         <v>7</v>
       </c>
       <c r="B270">
-        <v>22446</v>
-      </c>
-      <c r="C270" t="s">
-        <v>241</v>
+        <v>22442</v>
       </c>
       <c r="D270" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.45">
@@ -4472,10 +4472,10 @@
         <v>22446</v>
       </c>
       <c r="C271" t="s">
-        <v>278</v>
+        <v>241</v>
       </c>
       <c r="D271" t="s">
-        <v>285</v>
+        <v>209</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.45">
@@ -4483,13 +4483,13 @@
         <v>7</v>
       </c>
       <c r="B272">
-        <v>22587</v>
+        <v>22446</v>
       </c>
       <c r="C272" t="s">
         <v>278</v>
       </c>
       <c r="D272" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.45">
@@ -4497,13 +4497,13 @@
         <v>7</v>
       </c>
       <c r="B273">
-        <v>22588</v>
+        <v>22587</v>
       </c>
       <c r="C273" t="s">
         <v>278</v>
       </c>
       <c r="D273" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.45">
@@ -4511,13 +4511,13 @@
         <v>7</v>
       </c>
       <c r="B274">
-        <v>22589</v>
+        <v>22588</v>
       </c>
       <c r="C274" t="s">
         <v>278</v>
       </c>
       <c r="D274" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.45">
@@ -4525,13 +4525,13 @@
         <v>7</v>
       </c>
       <c r="B275">
-        <v>22590</v>
+        <v>22589</v>
       </c>
       <c r="C275" t="s">
         <v>278</v>
       </c>
       <c r="D275" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.45">
@@ -4539,13 +4539,13 @@
         <v>7</v>
       </c>
       <c r="B276">
-        <v>22591</v>
+        <v>22590</v>
       </c>
       <c r="C276" t="s">
         <v>278</v>
       </c>
       <c r="D276" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.45">
@@ -4553,13 +4553,13 @@
         <v>7</v>
       </c>
       <c r="B277">
-        <v>22592</v>
+        <v>22591</v>
       </c>
       <c r="C277" t="s">
         <v>278</v>
       </c>
       <c r="D277" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.45">
@@ -4567,13 +4567,13 @@
         <v>7</v>
       </c>
       <c r="B278">
-        <v>22593</v>
+        <v>22592</v>
       </c>
       <c r="C278" t="s">
         <v>278</v>
       </c>
       <c r="D278" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.45">
@@ -4581,13 +4581,13 @@
         <v>7</v>
       </c>
       <c r="B279">
-        <v>22594</v>
+        <v>22593</v>
       </c>
       <c r="C279" t="s">
         <v>278</v>
       </c>
       <c r="D279" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.45">
@@ -4595,13 +4595,13 @@
         <v>7</v>
       </c>
       <c r="B280">
-        <v>22595</v>
+        <v>22594</v>
       </c>
       <c r="C280" t="s">
         <v>278</v>
       </c>
       <c r="D280" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.45">
@@ -4609,38 +4609,41 @@
         <v>7</v>
       </c>
       <c r="B281">
-        <v>22596</v>
+        <v>22595</v>
       </c>
       <c r="C281" t="s">
         <v>278</v>
       </c>
       <c r="D281" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A282" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B282">
-        <v>26572</v>
+        <v>22596</v>
       </c>
       <c r="C282" t="s">
         <v>278</v>
       </c>
       <c r="D282" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A283" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B283">
-        <v>22447</v>
+        <v>26572</v>
+      </c>
+      <c r="C283" t="s">
+        <v>278</v>
       </c>
       <c r="D283" t="s">
-        <v>101</v>
+        <v>296</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.45">
@@ -4648,10 +4651,10 @@
         <v>7</v>
       </c>
       <c r="B284">
-        <v>22448</v>
+        <v>22447</v>
       </c>
       <c r="D284" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.45">
@@ -4659,13 +4662,10 @@
         <v>7</v>
       </c>
       <c r="B285">
-        <v>22450</v>
+        <v>22448</v>
       </c>
       <c r="D285" t="s">
-        <v>60</v>
-      </c>
-      <c r="E285" t="s">
-        <v>210</v>
+        <v>102</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.45">
@@ -4673,10 +4673,13 @@
         <v>7</v>
       </c>
       <c r="B286">
-        <v>22449</v>
+        <v>22450</v>
       </c>
       <c r="D286" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="E286" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.45">
@@ -4684,10 +4687,10 @@
         <v>7</v>
       </c>
       <c r="B287">
-        <v>22451</v>
+        <v>22449</v>
       </c>
       <c r="D287" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.45">
@@ -4695,10 +4698,10 @@
         <v>7</v>
       </c>
       <c r="B288">
-        <v>23737</v>
+        <v>22451</v>
       </c>
       <c r="D288" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.45">
@@ -4706,10 +4709,10 @@
         <v>7</v>
       </c>
       <c r="B289">
-        <v>22457</v>
+        <v>23737</v>
       </c>
       <c r="D289" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.45">
@@ -4717,10 +4720,10 @@
         <v>7</v>
       </c>
       <c r="B290">
-        <v>22456</v>
+        <v>22457</v>
       </c>
       <c r="D290" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.45">
@@ -4728,10 +4731,10 @@
         <v>7</v>
       </c>
       <c r="B291">
-        <v>24821</v>
+        <v>22456</v>
       </c>
       <c r="D291" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.45">
@@ -4739,10 +4742,10 @@
         <v>7</v>
       </c>
       <c r="B292">
-        <v>24822</v>
+        <v>24821</v>
       </c>
       <c r="D292" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.45">
@@ -4750,10 +4753,10 @@
         <v>7</v>
       </c>
       <c r="B293">
-        <v>22481</v>
+        <v>24822</v>
       </c>
       <c r="D293" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.45">
@@ -4761,10 +4764,10 @@
         <v>7</v>
       </c>
       <c r="B294">
-        <v>22479</v>
+        <v>22481</v>
       </c>
       <c r="D294" t="s">
-        <v>175</v>
+        <v>18</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.45">
@@ -4772,10 +4775,10 @@
         <v>7</v>
       </c>
       <c r="B295">
-        <v>22480</v>
+        <v>22479</v>
       </c>
       <c r="D295" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.45">
@@ -4783,10 +4786,10 @@
         <v>7</v>
       </c>
       <c r="B296">
-        <v>22467</v>
+        <v>22480</v>
       </c>
       <c r="D296" t="s">
-        <v>211</v>
+        <v>176</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.45">
@@ -4794,10 +4797,10 @@
         <v>7</v>
       </c>
       <c r="B297">
-        <v>22458</v>
+        <v>22467</v>
       </c>
       <c r="D297" t="s">
-        <v>103</v>
+        <v>211</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.45">
@@ -4805,10 +4808,10 @@
         <v>7</v>
       </c>
       <c r="B298">
-        <v>22462</v>
+        <v>22458</v>
       </c>
       <c r="D298" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.45">
@@ -4816,10 +4819,10 @@
         <v>7</v>
       </c>
       <c r="B299">
-        <v>22463</v>
+        <v>22462</v>
       </c>
       <c r="D299" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.45">
@@ -4827,10 +4830,10 @@
         <v>7</v>
       </c>
       <c r="B300">
-        <v>22464</v>
+        <v>22463</v>
       </c>
       <c r="D300" t="s">
-        <v>269</v>
+        <v>75</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.45">
@@ -4838,10 +4841,10 @@
         <v>7</v>
       </c>
       <c r="B301">
-        <v>22486</v>
+        <v>22464</v>
       </c>
       <c r="D301" t="s">
-        <v>26</v>
+        <v>269</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.45">
@@ -4849,10 +4852,10 @@
         <v>7</v>
       </c>
       <c r="B302">
-        <v>22465</v>
+        <v>22486</v>
       </c>
       <c r="D302" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.45">
@@ -4860,10 +4863,10 @@
         <v>7</v>
       </c>
       <c r="B303">
-        <v>22466</v>
+        <v>22465</v>
       </c>
       <c r="D303" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.45">
@@ -4871,10 +4874,10 @@
         <v>7</v>
       </c>
       <c r="B304">
-        <v>26461</v>
+        <v>22466</v>
       </c>
       <c r="D304" t="s">
-        <v>212</v>
+        <v>28</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.45">
@@ -4882,24 +4885,21 @@
         <v>7</v>
       </c>
       <c r="B305">
-        <v>26462</v>
+        <v>26461</v>
       </c>
       <c r="D305" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A306" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B306">
-        <v>24838</v>
+        <v>26462</v>
       </c>
       <c r="D306" t="s">
-        <v>215</v>
-      </c>
-      <c r="E306" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.45">
@@ -4907,10 +4907,13 @@
         <v>16</v>
       </c>
       <c r="B307">
-        <v>24842</v>
+        <v>24838</v>
       </c>
       <c r="D307" t="s">
-        <v>216</v>
+        <v>215</v>
+      </c>
+      <c r="E307" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.45">
@@ -4918,10 +4921,10 @@
         <v>16</v>
       </c>
       <c r="B308">
-        <v>24846</v>
+        <v>24842</v>
       </c>
       <c r="D308" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.45">
@@ -4929,10 +4932,10 @@
         <v>16</v>
       </c>
       <c r="B309">
-        <v>24849</v>
+        <v>24846</v>
       </c>
       <c r="D309" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.45">
@@ -4940,10 +4943,10 @@
         <v>16</v>
       </c>
       <c r="B310">
-        <v>24852</v>
+        <v>24849</v>
       </c>
       <c r="D310" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.45">
@@ -4951,10 +4954,10 @@
         <v>16</v>
       </c>
       <c r="B311">
-        <v>24856</v>
+        <v>24852</v>
       </c>
       <c r="D311" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.45">
@@ -4962,24 +4965,21 @@
         <v>16</v>
       </c>
       <c r="B312">
-        <v>24859</v>
+        <v>24856</v>
       </c>
       <c r="D312" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A313" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B313">
-        <v>7315</v>
+        <v>24859</v>
       </c>
       <c r="D313" t="s">
-        <v>223</v>
-      </c>
-      <c r="E313" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.45">
@@ -4987,21 +4987,24 @@
         <v>20</v>
       </c>
       <c r="B314">
-        <v>7316</v>
+        <v>7315</v>
       </c>
       <c r="D314" t="s">
-        <v>224</v>
+        <v>223</v>
+      </c>
+      <c r="E314" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A315" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B315">
-        <v>6818</v>
+        <v>7316</v>
       </c>
       <c r="D315" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.45">
@@ -5009,13 +5012,10 @@
         <v>7</v>
       </c>
       <c r="B316">
-        <v>23566</v>
+        <v>6818</v>
       </c>
       <c r="D316" t="s">
-        <v>231</v>
-      </c>
-      <c r="E316" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.45">
@@ -5023,10 +5023,13 @@
         <v>7</v>
       </c>
       <c r="B317">
-        <v>23567</v>
+        <v>23566</v>
       </c>
       <c r="D317" t="s">
-        <v>56</v>
+        <v>231</v>
+      </c>
+      <c r="E317" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.45">
@@ -5034,10 +5037,10 @@
         <v>7</v>
       </c>
       <c r="B318">
-        <v>24655</v>
+        <v>23567</v>
       </c>
       <c r="D318" t="s">
-        <v>232</v>
+        <v>56</v>
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.45">
@@ -5045,13 +5048,10 @@
         <v>7</v>
       </c>
       <c r="B319">
-        <v>23233</v>
+        <v>24655</v>
       </c>
       <c r="D319" t="s">
-        <v>271</v>
-      </c>
-      <c r="E319" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.45">
@@ -5059,10 +5059,13 @@
         <v>7</v>
       </c>
       <c r="B320">
-        <v>23234</v>
+        <v>23233</v>
       </c>
       <c r="D320" t="s">
-        <v>160</v>
+        <v>271</v>
+      </c>
+      <c r="E320" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.45">
@@ -5070,10 +5073,10 @@
         <v>7</v>
       </c>
       <c r="B321">
-        <v>23235</v>
+        <v>23234</v>
       </c>
       <c r="D321" t="s">
-        <v>56</v>
+        <v>160</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.45">
@@ -5081,10 +5084,10 @@
         <v>7</v>
       </c>
       <c r="B322">
-        <v>23240</v>
+        <v>23235</v>
       </c>
       <c r="D322" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.45">
@@ -5092,10 +5095,10 @@
         <v>7</v>
       </c>
       <c r="B323">
-        <v>23239</v>
+        <v>23240</v>
       </c>
       <c r="D323" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.45">
@@ -5103,10 +5106,10 @@
         <v>7</v>
       </c>
       <c r="B324">
-        <v>23237</v>
+        <v>23239</v>
       </c>
       <c r="D324" t="s">
-        <v>272</v>
+        <v>54</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.45">
@@ -5114,10 +5117,10 @@
         <v>7</v>
       </c>
       <c r="B325">
-        <v>23257</v>
+        <v>23237</v>
       </c>
       <c r="D325" t="s">
-        <v>177</v>
+        <v>272</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.45">
@@ -5125,10 +5128,10 @@
         <v>7</v>
       </c>
       <c r="B326">
-        <v>23251</v>
+        <v>23257</v>
       </c>
       <c r="D326" t="s">
-        <v>273</v>
+        <v>177</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.45">
@@ -5136,10 +5139,10 @@
         <v>7</v>
       </c>
       <c r="B327">
-        <v>23241</v>
+        <v>23251</v>
       </c>
       <c r="D327" t="s">
-        <v>68</v>
+        <v>273</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.45">
@@ -5147,10 +5150,10 @@
         <v>7</v>
       </c>
       <c r="B328">
-        <v>23242</v>
+        <v>23241</v>
       </c>
       <c r="D328" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.45">
@@ -5158,10 +5161,10 @@
         <v>7</v>
       </c>
       <c r="B329">
-        <v>23255</v>
+        <v>23242</v>
       </c>
       <c r="D329" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.45">
@@ -5169,10 +5172,10 @@
         <v>7</v>
       </c>
       <c r="B330">
-        <v>23254</v>
+        <v>23255</v>
       </c>
       <c r="D330" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.45">
@@ -5180,10 +5183,10 @@
         <v>7</v>
       </c>
       <c r="B331">
-        <v>23243</v>
+        <v>23254</v>
       </c>
       <c r="D331" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.45">
@@ -5191,20 +5194,31 @@
         <v>7</v>
       </c>
       <c r="B332">
-        <v>23244</v>
+        <v>23243</v>
       </c>
       <c r="D332" t="s">
-        <v>274</v>
+        <v>106</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A333" t="s">
+        <v>7</v>
+      </c>
+      <c r="B333">
+        <v>23244</v>
+      </c>
+      <c r="D333" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A334" t="s">
         <v>16</v>
       </c>
-      <c r="B333">
+      <c r="B334">
         <v>25019</v>
       </c>
-      <c r="D333" t="s">
+      <c r="D334" t="s">
         <v>301</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added labels for the contacts detail page.
</commit_message>
<xml_diff>
--- a/Controls.xlsx
+++ b/Controls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl-Otto\Documents\src\NVDA\vismaadministration-nvdaaddon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD5DCDA-92C2-436C-B12D-979F2E126C4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17267DD8-6A59-4B81-83D5-38F052A38512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="23040" windowHeight="12232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="30915" windowHeight="16876" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="306">
   <si>
     <t>WindowClassName</t>
   </si>
@@ -964,6 +964,15 @@
   </si>
   <si>
     <t>Kundfordranskonto</t>
+  </si>
+  <si>
+    <t>Titel</t>
+  </si>
+  <si>
+    <t>Företagsnamn</t>
+  </si>
+  <si>
+    <t>Postadress 2</t>
   </si>
 </sst>
 </file>
@@ -1281,10 +1290,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E334"/>
+  <dimension ref="A1:E352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
-      <selection activeCell="D212" sqref="D212"/>
+    <sheetView tabSelected="1" topLeftCell="A309" workbookViewId="0">
+      <selection activeCell="B352" sqref="B352:D352"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5222,6 +5231,258 @@
         <v>301</v>
       </c>
     </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A335" t="s">
+        <v>7</v>
+      </c>
+      <c r="B335">
+        <v>24695</v>
+      </c>
+      <c r="C335" t="s">
+        <v>248</v>
+      </c>
+      <c r="D335" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A336" t="s">
+        <v>7</v>
+      </c>
+      <c r="B336">
+        <v>24694</v>
+      </c>
+      <c r="C336" t="s">
+        <v>248</v>
+      </c>
+      <c r="D336" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A337" t="s">
+        <v>7</v>
+      </c>
+      <c r="B337">
+        <v>24696</v>
+      </c>
+      <c r="C337" t="s">
+        <v>248</v>
+      </c>
+      <c r="D337" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A338" t="s">
+        <v>7</v>
+      </c>
+      <c r="B338">
+        <v>24697</v>
+      </c>
+      <c r="C338" t="s">
+        <v>248</v>
+      </c>
+      <c r="D338" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A339" t="s">
+        <v>7</v>
+      </c>
+      <c r="B339">
+        <v>24698</v>
+      </c>
+      <c r="C339" t="s">
+        <v>248</v>
+      </c>
+      <c r="D339" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A340" t="s">
+        <v>7</v>
+      </c>
+      <c r="B340">
+        <v>24699</v>
+      </c>
+      <c r="C340" t="s">
+        <v>248</v>
+      </c>
+      <c r="D340" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A341" t="s">
+        <v>7</v>
+      </c>
+      <c r="B341">
+        <v>24700</v>
+      </c>
+      <c r="C341" t="s">
+        <v>248</v>
+      </c>
+      <c r="D341" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A342" t="s">
+        <v>7</v>
+      </c>
+      <c r="B342">
+        <v>24701</v>
+      </c>
+      <c r="C342" t="s">
+        <v>248</v>
+      </c>
+      <c r="D342" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A343" t="s">
+        <v>7</v>
+      </c>
+      <c r="B343">
+        <v>24702</v>
+      </c>
+      <c r="C343" t="s">
+        <v>248</v>
+      </c>
+      <c r="D343" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A344" t="s">
+        <v>7</v>
+      </c>
+      <c r="B344">
+        <v>24703</v>
+      </c>
+      <c r="C344" t="s">
+        <v>248</v>
+      </c>
+      <c r="D344" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A345" t="s">
+        <v>7</v>
+      </c>
+      <c r="B345">
+        <v>24704</v>
+      </c>
+      <c r="C345" t="s">
+        <v>248</v>
+      </c>
+      <c r="D345" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A346" t="s">
+        <v>7</v>
+      </c>
+      <c r="B346">
+        <v>24705</v>
+      </c>
+      <c r="C346" t="s">
+        <v>248</v>
+      </c>
+      <c r="D346" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A347" t="s">
+        <v>7</v>
+      </c>
+      <c r="B347">
+        <v>24707</v>
+      </c>
+      <c r="C347" t="s">
+        <v>248</v>
+      </c>
+      <c r="D347" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="348" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A348" t="s">
+        <v>7</v>
+      </c>
+      <c r="B348">
+        <v>24708</v>
+      </c>
+      <c r="C348" t="s">
+        <v>248</v>
+      </c>
+      <c r="D348" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="349" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A349" t="s">
+        <v>7</v>
+      </c>
+      <c r="B349">
+        <v>24709</v>
+      </c>
+      <c r="C349" t="s">
+        <v>248</v>
+      </c>
+      <c r="D349" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A350" t="s">
+        <v>7</v>
+      </c>
+      <c r="B350">
+        <v>24711</v>
+      </c>
+      <c r="C350" t="s">
+        <v>248</v>
+      </c>
+      <c r="D350" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="351" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A351" t="s">
+        <v>7</v>
+      </c>
+      <c r="B351">
+        <v>24710</v>
+      </c>
+      <c r="C351" t="s">
+        <v>248</v>
+      </c>
+      <c r="D351" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="352" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A352" t="s">
+        <v>7</v>
+      </c>
+      <c r="B352">
+        <v>24706</v>
+      </c>
+      <c r="C352" t="s">
+        <v>248</v>
+      </c>
+      <c r="D352" t="s">
+        <v>300</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added support fot the SysTabControl32 and SystemDialog so we get better speech output.
</commit_message>
<xml_diff>
--- a/Controls.xlsx
+++ b/Controls.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl-Otto\Documents\src\NVDA\vismaadministration-nvdaaddon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17267DD8-6A59-4B81-83D5-38F052A38512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6398529-362B-48B5-BF3D-F8CFB317C3A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="30915" windowHeight="16876" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="331">
   <si>
     <t>WindowClassName</t>
   </si>
@@ -973,6 +973,81 @@
   </si>
   <si>
     <t>Postadress 2</t>
+  </si>
+  <si>
+    <t>Kontoplan</t>
+  </si>
+  <si>
+    <t>Kontonummer</t>
+  </si>
+  <si>
+    <t>Momsrapportkod</t>
+  </si>
+  <si>
+    <t>Kontotyp</t>
+  </si>
+  <si>
+    <t>SRU-kod</t>
+  </si>
+  <si>
+    <t>Automatfördelning</t>
+  </si>
+  <si>
+    <t>Debet/Kredit</t>
+  </si>
+  <si>
+    <t>Motkonto</t>
+  </si>
+  <si>
+    <t>Föreslå följande resultatenhet</t>
+  </si>
+  <si>
+    <t>Föreslå följande projekt</t>
+  </si>
+  <si>
+    <t>Subkonto</t>
+  </si>
+  <si>
+    <t>Föreslå följande subkonto</t>
+  </si>
+  <si>
+    <t>Kvantitet</t>
+  </si>
+  <si>
+    <t>Föreslå följande kvantitet</t>
+  </si>
+  <si>
+    <t>Enhet för kvantitet</t>
+  </si>
+  <si>
+    <t>Transaktionsinfo</t>
+  </si>
+  <si>
+    <t>Föreslå följande transaktionsinfo</t>
+  </si>
+  <si>
+    <t>Periodisering</t>
+  </si>
+  <si>
+    <t>Första periodiseringsdatum</t>
+  </si>
+  <si>
+    <t>Delas på antal månader</t>
+  </si>
+  <si>
+    <t>Verifikationsserie</t>
+  </si>
+  <si>
+    <t>Verifikationstext</t>
+  </si>
+  <si>
+    <t>Intäktskonto</t>
+  </si>
+  <si>
+    <t>Periodiseringskonto</t>
+  </si>
+  <si>
+    <t>Namn på periodiseringen</t>
   </si>
 </sst>
 </file>
@@ -1290,10 +1365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E352"/>
+  <dimension ref="A1:E380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A309" workbookViewId="0">
-      <selection activeCell="B352" sqref="B352:D352"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A380" sqref="A1:E380"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5483,6 +5558,398 @@
         <v>300</v>
       </c>
     </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A353" t="s">
+        <v>7</v>
+      </c>
+      <c r="B353">
+        <v>22175</v>
+      </c>
+      <c r="C353" t="s">
+        <v>306</v>
+      </c>
+      <c r="D353" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A354" t="s">
+        <v>7</v>
+      </c>
+      <c r="B354">
+        <v>22176</v>
+      </c>
+      <c r="C354" t="s">
+        <v>306</v>
+      </c>
+      <c r="D354" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="355" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A355" t="s">
+        <v>16</v>
+      </c>
+      <c r="B355">
+        <v>22177</v>
+      </c>
+      <c r="C355" t="s">
+        <v>306</v>
+      </c>
+      <c r="D355" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="356" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A356" t="s">
+        <v>16</v>
+      </c>
+      <c r="B356">
+        <v>23591</v>
+      </c>
+      <c r="C356" t="s">
+        <v>306</v>
+      </c>
+      <c r="D356" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="357" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A357" t="s">
+        <v>7</v>
+      </c>
+      <c r="B357">
+        <v>22178</v>
+      </c>
+      <c r="C357" t="s">
+        <v>306</v>
+      </c>
+      <c r="D357" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="358" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A358" t="s">
+        <v>7</v>
+      </c>
+      <c r="B358">
+        <v>22180</v>
+      </c>
+      <c r="C358" t="s">
+        <v>306</v>
+      </c>
+      <c r="D358" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="359" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A359" t="s">
+        <v>16</v>
+      </c>
+      <c r="B359">
+        <v>22179</v>
+      </c>
+      <c r="C359" t="s">
+        <v>306</v>
+      </c>
+      <c r="D359" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="360" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A360" t="s">
+        <v>7</v>
+      </c>
+      <c r="B360">
+        <v>24903</v>
+      </c>
+      <c r="C360" t="s">
+        <v>306</v>
+      </c>
+      <c r="D360" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="361" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A361" t="s">
+        <v>16</v>
+      </c>
+      <c r="B361">
+        <v>22183</v>
+      </c>
+      <c r="C361" t="s">
+        <v>306</v>
+      </c>
+      <c r="D361" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="362" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A362" t="s">
+        <v>7</v>
+      </c>
+      <c r="B362">
+        <v>22185</v>
+      </c>
+      <c r="C362" t="s">
+        <v>306</v>
+      </c>
+      <c r="D362" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="363" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A363" t="s">
+        <v>16</v>
+      </c>
+      <c r="B363">
+        <v>22186</v>
+      </c>
+      <c r="C363" t="s">
+        <v>306</v>
+      </c>
+      <c r="D363" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="364" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A364" t="s">
+        <v>7</v>
+      </c>
+      <c r="B364">
+        <v>22188</v>
+      </c>
+      <c r="C364" t="s">
+        <v>306</v>
+      </c>
+      <c r="D364" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="365" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A365" t="s">
+        <v>16</v>
+      </c>
+      <c r="B365">
+        <v>22189</v>
+      </c>
+      <c r="C365" t="s">
+        <v>306</v>
+      </c>
+      <c r="D365" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="366" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A366" t="s">
+        <v>7</v>
+      </c>
+      <c r="B366">
+        <v>22191</v>
+      </c>
+      <c r="C366" t="s">
+        <v>306</v>
+      </c>
+      <c r="D366" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="367" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A367" t="s">
+        <v>16</v>
+      </c>
+      <c r="B367">
+        <v>22192</v>
+      </c>
+      <c r="C367" t="s">
+        <v>306</v>
+      </c>
+      <c r="D367" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="368" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A368" t="s">
+        <v>7</v>
+      </c>
+      <c r="B368">
+        <v>22194</v>
+      </c>
+      <c r="C368" t="s">
+        <v>306</v>
+      </c>
+      <c r="D368" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="369" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A369" t="s">
+        <v>7</v>
+      </c>
+      <c r="B369">
+        <v>22195</v>
+      </c>
+      <c r="C369" t="s">
+        <v>306</v>
+      </c>
+      <c r="D369" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="370" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A370" t="s">
+        <v>16</v>
+      </c>
+      <c r="B370">
+        <v>22196</v>
+      </c>
+      <c r="C370" t="s">
+        <v>306</v>
+      </c>
+      <c r="D370" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="371" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A371" t="s">
+        <v>7</v>
+      </c>
+      <c r="B371">
+        <v>22198</v>
+      </c>
+      <c r="C371" t="s">
+        <v>306</v>
+      </c>
+      <c r="D371" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="372" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A372" t="s">
+        <v>7</v>
+      </c>
+      <c r="B372">
+        <v>22301</v>
+      </c>
+      <c r="C372" t="s">
+        <v>323</v>
+      </c>
+      <c r="D372" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="373" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A373" t="s">
+        <v>7</v>
+      </c>
+      <c r="B373">
+        <v>21164</v>
+      </c>
+      <c r="C373" t="s">
+        <v>323</v>
+      </c>
+      <c r="D373" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="374" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A374" t="s">
+        <v>7</v>
+      </c>
+      <c r="B374">
+        <v>21167</v>
+      </c>
+      <c r="C374" t="s">
+        <v>323</v>
+      </c>
+      <c r="D374" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="375" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A375" t="s">
+        <v>16</v>
+      </c>
+      <c r="B375">
+        <v>22303</v>
+      </c>
+      <c r="C375" t="s">
+        <v>323</v>
+      </c>
+      <c r="D375" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="376" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A376" t="s">
+        <v>7</v>
+      </c>
+      <c r="B376">
+        <v>22302</v>
+      </c>
+      <c r="C376" t="s">
+        <v>323</v>
+      </c>
+      <c r="D376" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="377" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A377" t="s">
+        <v>7</v>
+      </c>
+      <c r="B377">
+        <v>26470</v>
+      </c>
+      <c r="C377" t="s">
+        <v>323</v>
+      </c>
+      <c r="D377" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="378" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A378" t="s">
+        <v>7</v>
+      </c>
+      <c r="B378">
+        <v>24897</v>
+      </c>
+      <c r="C378" t="s">
+        <v>323</v>
+      </c>
+      <c r="D378" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="379" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A379" t="s">
+        <v>7</v>
+      </c>
+      <c r="B379">
+        <v>24894</v>
+      </c>
+      <c r="C379" t="s">
+        <v>323</v>
+      </c>
+      <c r="D379" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="380" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A380" t="s">
+        <v>7</v>
+      </c>
+      <c r="B380">
+        <v>24895</v>
+      </c>
+      <c r="C380" t="s">
+        <v>323</v>
+      </c>
+      <c r="D380" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added support for mass update. Problem is that it's the same control ids and the module doesn't seem to filter that unfortunately. Have to check that.
</commit_message>
<xml_diff>
--- a/Controls.xlsx
+++ b/Controls.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl-Otto\Documents\src\NVDA\vismaadministration-nvdaaddon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6398529-362B-48B5-BF3D-F8CFB317C3A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F797501-70BE-4B7F-BCEF-465D055EEB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="30915" windowHeight="16876" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="401">
   <si>
     <t>WindowClassName</t>
   </si>
@@ -1048,6 +1048,216 @@
   </si>
   <si>
     <t>Namn på periodiseringen</t>
+  </si>
+  <si>
+    <t>Lås upp Inaktivera</t>
+  </si>
+  <si>
+    <t>Lås upp Landskod</t>
+  </si>
+  <si>
+    <t>Lås upp Landskod leveransadress</t>
+  </si>
+  <si>
+    <t>Lås upp Kundkategori</t>
+  </si>
+  <si>
+    <t>Lås upp Distrikt</t>
+  </si>
+  <si>
+    <t>Lås upp Säljare</t>
+  </si>
+  <si>
+    <t>Lås up Leveranssätt</t>
+  </si>
+  <si>
+    <t>Lås upp Speditör</t>
+  </si>
+  <si>
+    <t>Lås upp Språk</t>
+  </si>
+  <si>
+    <t>Lås upp Valuta</t>
+  </si>
+  <si>
+    <t>Lås upp Sorteringsbegrepp</t>
+  </si>
+  <si>
+    <t>Lås upp Kreditgräns kronor</t>
+  </si>
+  <si>
+    <t>Lås upp Export</t>
+  </si>
+  <si>
+    <t>Lås upp EU-kund</t>
+  </si>
+  <si>
+    <t>Lås upp Räntefakturering</t>
+  </si>
+  <si>
+    <t>Lås upp Betalningspåminnelse</t>
+  </si>
+  <si>
+    <t>Lås upp Påminnelseavgift</t>
+  </si>
+  <si>
+    <t>Lås upp Restnotera ej</t>
+  </si>
+  <si>
+    <t>Lås upp Expeditionsavgift</t>
+  </si>
+  <si>
+    <t>Lås upp Frakt</t>
+  </si>
+  <si>
+    <t>Lås upp Intrastat</t>
+  </si>
+  <si>
+    <t>Lås upp Samlingsfakturering</t>
+  </si>
+  <si>
+    <t>Lås upp Överför adress till beställning</t>
+  </si>
+  <si>
+    <t>Lås upp Anmärkning 1</t>
+  </si>
+  <si>
+    <t>Lås upp Anmärkning 2</t>
+  </si>
+  <si>
+    <t>Lås upp Rabattavtal</t>
+  </si>
+  <si>
+    <t>Lås upp Betalningsvillkor</t>
+  </si>
+  <si>
+    <t>Lås upp Prislista</t>
+  </si>
+  <si>
+    <t>Lås upp Fakturarabatt i %</t>
+  </si>
+  <si>
+    <t>Lås upp Radrabatt</t>
+  </si>
+  <si>
+    <t>Lås upp Leveransvillkor</t>
+  </si>
+  <si>
+    <t>Lås upp Kundfordranskonto</t>
+  </si>
+  <si>
+    <t>Lås upp Offert</t>
+  </si>
+  <si>
+    <t>Lås upp Order</t>
+  </si>
+  <si>
+    <t>Lås upp Följesedel</t>
+  </si>
+  <si>
+    <t>Lås upp Extra orderdokument</t>
+  </si>
+  <si>
+    <t>Lås upp Faktura</t>
+  </si>
+  <si>
+    <t>Lås upp Extra fakturadokument</t>
+  </si>
+  <si>
+    <t>Lås upp Kopia Offert</t>
+  </si>
+  <si>
+    <t>Kopia Offert</t>
+  </si>
+  <si>
+    <t>Lås upp Kopia Order</t>
+  </si>
+  <si>
+    <t>Kopia Order</t>
+  </si>
+  <si>
+    <t>Lås upp Kopia Följesedel</t>
+  </si>
+  <si>
+    <t>Kopia Följesedel</t>
+  </si>
+  <si>
+    <t>Lås upp Kopia Extra orderdokument</t>
+  </si>
+  <si>
+    <t>Kopia Extra orderdokument</t>
+  </si>
+  <si>
+    <t>Lås upp Kopia Faktura</t>
+  </si>
+  <si>
+    <t>Kopia Faktura</t>
+  </si>
+  <si>
+    <t>Lås upp Kopia Kreditfaktura</t>
+  </si>
+  <si>
+    <t>Kopia Kreditfaktura</t>
+  </si>
+  <si>
+    <t>Lås upp Kopia Räntefaktura</t>
+  </si>
+  <si>
+    <t>Kopia Räntefaktura</t>
+  </si>
+  <si>
+    <t>Lås upp Kopia Kontantnota</t>
+  </si>
+  <si>
+    <t>Kopia Kontantnota</t>
+  </si>
+  <si>
+    <t>Lås upp Kopia Extra fakturadokument</t>
+  </si>
+  <si>
+    <t>Kopia Extra fakturadokument</t>
+  </si>
+  <si>
+    <t>Lås upp Dokumentmall Faktura</t>
+  </si>
+  <si>
+    <t>Lås upp Dokumentmall Kreditfaktura</t>
+  </si>
+  <si>
+    <t>Lås upp Dokumentmall Räntefaktura</t>
+  </si>
+  <si>
+    <t>Lås upp Dokumentmall Kontantnota</t>
+  </si>
+  <si>
+    <t>Lås upp Dokumentmall Extra fakturadokument</t>
+  </si>
+  <si>
+    <t>Lås upp Utskriftsval Offert</t>
+  </si>
+  <si>
+    <t>Lås upp Utskriftsval Order</t>
+  </si>
+  <si>
+    <t>Lås upp Utskriftsval Följesedel</t>
+  </si>
+  <si>
+    <t>Lås upp Utskriftsval Extra orderdokument</t>
+  </si>
+  <si>
+    <t>Lås upp Utskriftsval Faktura</t>
+  </si>
+  <si>
+    <t>Lås upp Utskriftsval Kreditfaktura</t>
+  </si>
+  <si>
+    <t>Lås upp Utskriftsval Räntefaktura</t>
+  </si>
+  <si>
+    <t>Lås upp Utskriftsval Kontantnota</t>
+  </si>
+  <si>
+    <t>Lås upp Utskriftsval Extra fakturadokument</t>
   </si>
 </sst>
 </file>
@@ -1365,10 +1575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E380"/>
+  <dimension ref="A1:E451"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A380" sqref="A1:E380"/>
+    <sheetView tabSelected="1" topLeftCell="A409" workbookViewId="0">
+      <selection activeCell="C451" sqref="C451"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5950,6 +6160,1000 @@
         <v>65</v>
       </c>
     </row>
+    <row r="381" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A381" t="s">
+        <v>20</v>
+      </c>
+      <c r="B381">
+        <v>25052</v>
+      </c>
+      <c r="C381" t="s">
+        <v>241</v>
+      </c>
+      <c r="D381" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A382" t="s">
+        <v>20</v>
+      </c>
+      <c r="B382">
+        <v>23978</v>
+      </c>
+      <c r="C382" t="s">
+        <v>241</v>
+      </c>
+      <c r="D382" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="383" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A383" t="s">
+        <v>20</v>
+      </c>
+      <c r="B383">
+        <v>23983</v>
+      </c>
+      <c r="C383" t="s">
+        <v>241</v>
+      </c>
+      <c r="D383" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="384" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A384" t="s">
+        <v>20</v>
+      </c>
+      <c r="B384">
+        <v>23868</v>
+      </c>
+      <c r="C384" t="s">
+        <v>241</v>
+      </c>
+      <c r="D384" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="385" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A385" t="s">
+        <v>20</v>
+      </c>
+      <c r="B385">
+        <v>23869</v>
+      </c>
+      <c r="C385" t="s">
+        <v>241</v>
+      </c>
+      <c r="D385" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="386" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A386" t="s">
+        <v>20</v>
+      </c>
+      <c r="B386">
+        <v>23870</v>
+      </c>
+      <c r="C386" t="s">
+        <v>241</v>
+      </c>
+      <c r="D386" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="387" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A387" t="s">
+        <v>20</v>
+      </c>
+      <c r="B387">
+        <v>23873</v>
+      </c>
+      <c r="C387" t="s">
+        <v>241</v>
+      </c>
+      <c r="D387" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="388" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A388" t="s">
+        <v>20</v>
+      </c>
+      <c r="B388">
+        <v>23874</v>
+      </c>
+      <c r="C388" t="s">
+        <v>241</v>
+      </c>
+      <c r="D388" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="389" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A389" t="s">
+        <v>20</v>
+      </c>
+      <c r="B389">
+        <v>23875</v>
+      </c>
+      <c r="C389" t="s">
+        <v>241</v>
+      </c>
+      <c r="D389" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A390" t="s">
+        <v>20</v>
+      </c>
+      <c r="B390">
+        <v>23876</v>
+      </c>
+      <c r="C390" t="s">
+        <v>241</v>
+      </c>
+      <c r="D390" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A391" t="s">
+        <v>20</v>
+      </c>
+      <c r="B391">
+        <v>23877</v>
+      </c>
+      <c r="C391" t="s">
+        <v>241</v>
+      </c>
+      <c r="D391" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="392" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A392" t="s">
+        <v>20</v>
+      </c>
+      <c r="B392">
+        <v>23878</v>
+      </c>
+      <c r="C392" t="s">
+        <v>241</v>
+      </c>
+      <c r="D392" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="393" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A393" t="s">
+        <v>20</v>
+      </c>
+      <c r="B393">
+        <v>23879</v>
+      </c>
+      <c r="C393" t="s">
+        <v>241</v>
+      </c>
+      <c r="D393" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="394" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A394" t="s">
+        <v>20</v>
+      </c>
+      <c r="B394">
+        <v>23880</v>
+      </c>
+      <c r="C394" t="s">
+        <v>241</v>
+      </c>
+      <c r="D394" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="395" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A395" t="s">
+        <v>20</v>
+      </c>
+      <c r="B395">
+        <v>23881</v>
+      </c>
+      <c r="C395" t="s">
+        <v>241</v>
+      </c>
+      <c r="D395" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="396" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A396" t="s">
+        <v>20</v>
+      </c>
+      <c r="B396">
+        <v>23882</v>
+      </c>
+      <c r="C396" t="s">
+        <v>241</v>
+      </c>
+      <c r="D396" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A397" t="s">
+        <v>20</v>
+      </c>
+      <c r="B397">
+        <v>23883</v>
+      </c>
+      <c r="C397" t="s">
+        <v>241</v>
+      </c>
+      <c r="D397" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="398" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A398" t="s">
+        <v>20</v>
+      </c>
+      <c r="B398">
+        <v>23884</v>
+      </c>
+      <c r="C398" t="s">
+        <v>241</v>
+      </c>
+      <c r="D398" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="399" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A399" t="s">
+        <v>20</v>
+      </c>
+      <c r="B399">
+        <v>23885</v>
+      </c>
+      <c r="C399" t="s">
+        <v>241</v>
+      </c>
+      <c r="D399" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="400" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A400" t="s">
+        <v>20</v>
+      </c>
+      <c r="B400">
+        <v>23886</v>
+      </c>
+      <c r="C400" t="s">
+        <v>241</v>
+      </c>
+      <c r="D400" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="401" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A401" t="s">
+        <v>20</v>
+      </c>
+      <c r="B401">
+        <v>26659</v>
+      </c>
+      <c r="C401" t="s">
+        <v>241</v>
+      </c>
+      <c r="D401" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="402" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A402" t="s">
+        <v>20</v>
+      </c>
+      <c r="B402">
+        <v>23887</v>
+      </c>
+      <c r="C402" t="s">
+        <v>241</v>
+      </c>
+      <c r="D402" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="403" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A403" t="s">
+        <v>20</v>
+      </c>
+      <c r="B403">
+        <v>24123</v>
+      </c>
+      <c r="C403" t="s">
+        <v>241</v>
+      </c>
+      <c r="D403" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="404" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A404" t="s">
+        <v>20</v>
+      </c>
+      <c r="B404">
+        <v>26202</v>
+      </c>
+      <c r="C404" t="s">
+        <v>241</v>
+      </c>
+      <c r="D404" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="405" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A405" t="s">
+        <v>20</v>
+      </c>
+      <c r="B405">
+        <v>26203</v>
+      </c>
+      <c r="C405" t="s">
+        <v>241</v>
+      </c>
+      <c r="D405" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A406" t="s">
+        <v>20</v>
+      </c>
+      <c r="B406">
+        <v>23888</v>
+      </c>
+      <c r="C406" t="s">
+        <v>241</v>
+      </c>
+      <c r="D406" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="407" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A407" t="s">
+        <v>20</v>
+      </c>
+      <c r="B407">
+        <v>23871</v>
+      </c>
+      <c r="C407" t="s">
+        <v>241</v>
+      </c>
+      <c r="D407" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="408" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A408" t="s">
+        <v>20</v>
+      </c>
+      <c r="B408">
+        <v>23872</v>
+      </c>
+      <c r="C408" t="s">
+        <v>241</v>
+      </c>
+      <c r="D408" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="409" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A409" t="s">
+        <v>20</v>
+      </c>
+      <c r="B409">
+        <v>24088</v>
+      </c>
+      <c r="C409" t="s">
+        <v>241</v>
+      </c>
+      <c r="D409" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="410" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A410" t="s">
+        <v>20</v>
+      </c>
+      <c r="B410">
+        <v>23889</v>
+      </c>
+      <c r="C410" t="s">
+        <v>241</v>
+      </c>
+      <c r="D410" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="411" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A411" t="s">
+        <v>20</v>
+      </c>
+      <c r="B411">
+        <v>23890</v>
+      </c>
+      <c r="C411" t="s">
+        <v>241</v>
+      </c>
+      <c r="D411" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A412" t="s">
+        <v>20</v>
+      </c>
+      <c r="B412">
+        <v>23891</v>
+      </c>
+      <c r="C412" t="s">
+        <v>241</v>
+      </c>
+      <c r="D412" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A413" t="s">
+        <v>20</v>
+      </c>
+      <c r="B413">
+        <v>24873</v>
+      </c>
+      <c r="C413" t="s">
+        <v>241</v>
+      </c>
+      <c r="D413" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="414" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A414" t="s">
+        <v>20</v>
+      </c>
+      <c r="B414">
+        <v>24874</v>
+      </c>
+      <c r="C414" t="s">
+        <v>241</v>
+      </c>
+      <c r="D414" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="415" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A415" t="s">
+        <v>20</v>
+      </c>
+      <c r="B415">
+        <v>24875</v>
+      </c>
+      <c r="C415" t="s">
+        <v>241</v>
+      </c>
+      <c r="D415" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="416" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A416" t="s">
+        <v>20</v>
+      </c>
+      <c r="B416">
+        <v>24876</v>
+      </c>
+      <c r="C416" t="s">
+        <v>241</v>
+      </c>
+      <c r="D416" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="417" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A417" t="s">
+        <v>20</v>
+      </c>
+      <c r="B417">
+        <v>24877</v>
+      </c>
+      <c r="C417" t="s">
+        <v>241</v>
+      </c>
+      <c r="D417" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="418" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A418" t="s">
+        <v>20</v>
+      </c>
+      <c r="B418">
+        <v>24878</v>
+      </c>
+      <c r="C418" t="s">
+        <v>241</v>
+      </c>
+      <c r="D418" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="419" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A419" t="s">
+        <v>20</v>
+      </c>
+      <c r="B419">
+        <v>24879</v>
+      </c>
+      <c r="C419" t="s">
+        <v>241</v>
+      </c>
+      <c r="D419" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="420" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A420" t="s">
+        <v>20</v>
+      </c>
+      <c r="B420">
+        <v>24089</v>
+      </c>
+      <c r="C420" t="s">
+        <v>241</v>
+      </c>
+      <c r="D420" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="421" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A421" t="s">
+        <v>20</v>
+      </c>
+      <c r="B421">
+        <v>23892</v>
+      </c>
+      <c r="C421" t="s">
+        <v>241</v>
+      </c>
+      <c r="D421" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="422" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A422" t="s">
+        <v>20</v>
+      </c>
+      <c r="B422">
+        <v>24095</v>
+      </c>
+      <c r="C422" t="s">
+        <v>241</v>
+      </c>
+      <c r="D422" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="423" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A423" t="s">
+        <v>20</v>
+      </c>
+      <c r="B423">
+        <v>24174</v>
+      </c>
+      <c r="C423" t="s">
+        <v>241</v>
+      </c>
+      <c r="D423" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="424" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A424" t="s">
+        <v>20</v>
+      </c>
+      <c r="B424">
+        <v>23893</v>
+      </c>
+      <c r="C424" t="s">
+        <v>241</v>
+      </c>
+      <c r="D424" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A425" t="s">
+        <v>20</v>
+      </c>
+      <c r="B425">
+        <v>23894</v>
+      </c>
+      <c r="C425" t="s">
+        <v>241</v>
+      </c>
+      <c r="D425" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A426" t="s">
+        <v>20</v>
+      </c>
+      <c r="B426">
+        <v>23895</v>
+      </c>
+      <c r="C426" t="s">
+        <v>241</v>
+      </c>
+      <c r="D426" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="427" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A427" t="s">
+        <v>20</v>
+      </c>
+      <c r="B427">
+        <v>23984</v>
+      </c>
+      <c r="C427" t="s">
+        <v>241</v>
+      </c>
+      <c r="D427" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A428" t="s">
+        <v>20</v>
+      </c>
+      <c r="B428">
+        <v>23985</v>
+      </c>
+      <c r="C428" t="s">
+        <v>241</v>
+      </c>
+      <c r="D428" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A429" t="s">
+        <v>20</v>
+      </c>
+      <c r="B429">
+        <v>24090</v>
+      </c>
+      <c r="C429" t="s">
+        <v>241</v>
+      </c>
+      <c r="D429" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A430" t="s">
+        <v>7</v>
+      </c>
+      <c r="B430">
+        <v>25007</v>
+      </c>
+      <c r="C430" t="s">
+        <v>241</v>
+      </c>
+      <c r="D430" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A431" t="s">
+        <v>20</v>
+      </c>
+      <c r="B431">
+        <v>23988</v>
+      </c>
+      <c r="C431" t="s">
+        <v>241</v>
+      </c>
+      <c r="D431" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="432" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A432" t="s">
+        <v>7</v>
+      </c>
+      <c r="B432">
+        <v>24038</v>
+      </c>
+      <c r="C432" t="s">
+        <v>241</v>
+      </c>
+      <c r="D432" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A433" t="s">
+        <v>20</v>
+      </c>
+      <c r="B433">
+        <v>23987</v>
+      </c>
+      <c r="C433" t="s">
+        <v>241</v>
+      </c>
+      <c r="D433" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A434" t="s">
+        <v>7</v>
+      </c>
+      <c r="B434">
+        <v>25003</v>
+      </c>
+      <c r="C434" t="s">
+        <v>241</v>
+      </c>
+      <c r="D434" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A435" t="s">
+        <v>20</v>
+      </c>
+      <c r="B435">
+        <v>24085</v>
+      </c>
+      <c r="C435" t="s">
+        <v>241</v>
+      </c>
+      <c r="D435" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="436" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A436" t="s">
+        <v>7</v>
+      </c>
+      <c r="B436">
+        <v>25004</v>
+      </c>
+      <c r="C436" t="s">
+        <v>241</v>
+      </c>
+      <c r="D436" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="437" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A437" t="s">
+        <v>20</v>
+      </c>
+      <c r="B437">
+        <v>23989</v>
+      </c>
+      <c r="C437" t="s">
+        <v>241</v>
+      </c>
+      <c r="D437" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="438" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A438" t="s">
+        <v>7</v>
+      </c>
+      <c r="B438">
+        <v>24032</v>
+      </c>
+      <c r="C438" t="s">
+        <v>241</v>
+      </c>
+      <c r="D438" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A439" t="s">
+        <v>20</v>
+      </c>
+      <c r="B439">
+        <v>23990</v>
+      </c>
+      <c r="C439" t="s">
+        <v>241</v>
+      </c>
+      <c r="D439" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A440" t="s">
+        <v>7</v>
+      </c>
+      <c r="B440">
+        <v>24034</v>
+      </c>
+      <c r="C440" t="s">
+        <v>241</v>
+      </c>
+      <c r="D440" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A441" t="s">
+        <v>20</v>
+      </c>
+      <c r="B441">
+        <v>23991</v>
+      </c>
+      <c r="C441" t="s">
+        <v>241</v>
+      </c>
+      <c r="D441" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A442" t="s">
+        <v>7</v>
+      </c>
+      <c r="B442">
+        <v>24036</v>
+      </c>
+      <c r="C442" t="s">
+        <v>241</v>
+      </c>
+      <c r="D442" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A443" t="s">
+        <v>20</v>
+      </c>
+      <c r="B443">
+        <v>24086</v>
+      </c>
+      <c r="C443" t="s">
+        <v>241</v>
+      </c>
+      <c r="D443" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="444" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A444" t="s">
+        <v>7</v>
+      </c>
+      <c r="B444">
+        <v>25005</v>
+      </c>
+      <c r="C444" t="s">
+        <v>241</v>
+      </c>
+      <c r="D444" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A445" t="s">
+        <v>20</v>
+      </c>
+      <c r="B445">
+        <v>24087</v>
+      </c>
+      <c r="C445" t="s">
+        <v>241</v>
+      </c>
+      <c r="D445" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A446" t="s">
+        <v>7</v>
+      </c>
+      <c r="B446">
+        <v>25006</v>
+      </c>
+      <c r="C446" t="s">
+        <v>241</v>
+      </c>
+      <c r="D446" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A447" t="s">
+        <v>20</v>
+      </c>
+      <c r="B447">
+        <v>23986</v>
+      </c>
+      <c r="C447" t="s">
+        <v>241</v>
+      </c>
+      <c r="D447" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A448" t="s">
+        <v>20</v>
+      </c>
+      <c r="B448">
+        <v>24092</v>
+      </c>
+      <c r="C448" t="s">
+        <v>241</v>
+      </c>
+      <c r="D448" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="449" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A449" t="s">
+        <v>20</v>
+      </c>
+      <c r="B449">
+        <v>24093</v>
+      </c>
+      <c r="C449" t="s">
+        <v>241</v>
+      </c>
+      <c r="D449" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="450" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A450" t="s">
+        <v>20</v>
+      </c>
+      <c r="B450">
+        <v>24094</v>
+      </c>
+      <c r="C450" t="s">
+        <v>241</v>
+      </c>
+      <c r="D450" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A451" t="s">
+        <v>20</v>
+      </c>
+      <c r="B451">
+        <v>23896</v>
+      </c>
+      <c r="C451" t="s">
+        <v>241</v>
+      </c>
+      <c r="D451" t="s">
+        <v>391</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed some issues with getting the module name. Added verification controls.
</commit_message>
<xml_diff>
--- a/Controls.xlsx
+++ b/Controls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl-Otto\Documents\src\NVDA\vismaadministration-nvdaaddon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F797501-70BE-4B7F-BCEF-465D055EEB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100EE278-E9AB-4BFF-BB07-51918DF9D4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="30915" windowHeight="16876" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1073" yWindow="1073" windowWidth="23039" windowHeight="12232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="405">
   <si>
     <t>WindowClassName</t>
   </si>
@@ -1258,6 +1258,18 @@
   </si>
   <si>
     <t>Lås upp Utskriftsval Extra fakturadokument</t>
+  </si>
+  <si>
+    <t>Verifikationer</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Verifikationsrader</t>
+  </si>
+  <si>
+    <t>Verifikationslista</t>
   </si>
 </sst>
 </file>
@@ -1575,13 +1587,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E451"/>
+  <dimension ref="A1:E455"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A409" workbookViewId="0">
-      <selection activeCell="C451" sqref="C451"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A455" sqref="A1:E455"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="26.06640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
@@ -7154,6 +7169,62 @@
         <v>391</v>
       </c>
     </row>
+    <row r="452" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A452" t="s">
+        <v>7</v>
+      </c>
+      <c r="B452">
+        <v>22248</v>
+      </c>
+      <c r="C452" t="s">
+        <v>401</v>
+      </c>
+      <c r="D452" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A453" t="s">
+        <v>7</v>
+      </c>
+      <c r="B453">
+        <v>22251</v>
+      </c>
+      <c r="C453" t="s">
+        <v>401</v>
+      </c>
+      <c r="D453" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="454" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A454" t="s">
+        <v>29</v>
+      </c>
+      <c r="B454">
+        <v>20743</v>
+      </c>
+      <c r="C454" t="s">
+        <v>401</v>
+      </c>
+      <c r="D454" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A455" t="s">
+        <v>29</v>
+      </c>
+      <c r="B455">
+        <v>20723</v>
+      </c>
+      <c r="C455" t="s">
+        <v>401</v>
+      </c>
+      <c r="D455" t="s">
+        <v>404</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cleaned up the code so the module fetching works as expected. New modules are written as a line in the log and returned so we can use it immediately. Added a new control.
</commit_message>
<xml_diff>
--- a/Controls.xlsx
+++ b/Controls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl-Otto\Documents\src\NVDA\vismaadministration-nvdaaddon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100EE278-E9AB-4BFF-BB07-51918DF9D4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A68E98-F1A6-4851-A5DF-1B0199E97BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1073" yWindow="1073" windowWidth="23039" windowHeight="12232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1410" yWindow="1410" windowWidth="23040" windowHeight="12232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="423">
   <si>
     <t>WindowClassName</t>
   </si>
@@ -1270,6 +1270,60 @@
   </si>
   <si>
     <t>Verifikationslista</t>
+  </si>
+  <si>
+    <t>Konteringsmallar</t>
+  </si>
+  <si>
+    <t>Minus</t>
+  </si>
+  <si>
+    <t>Plus</t>
+  </si>
+  <si>
+    <t>Dividera</t>
+  </si>
+  <si>
+    <t>Multiplicera</t>
+  </si>
+  <si>
+    <t>Vänster parentes</t>
+  </si>
+  <si>
+    <t>Höger parentes</t>
+  </si>
+  <si>
+    <t>Vänster klammer</t>
+  </si>
+  <si>
+    <t>Höger klammer</t>
+  </si>
+  <si>
+    <t>Gamla journaler</t>
+  </si>
+  <si>
+    <t>Journaler</t>
+  </si>
+  <si>
+    <t>Momskontroll</t>
+  </si>
+  <si>
+    <t>Till och med</t>
+  </si>
+  <si>
+    <t>Från och med</t>
+  </si>
+  <si>
+    <t>Periodiseringar</t>
+  </si>
+  <si>
+    <t>Lista över periodiseringar</t>
+  </si>
+  <si>
+    <t>Fakturahantering</t>
+  </si>
+  <si>
+    <t>Fakturor</t>
   </si>
 </sst>
 </file>
@@ -1587,10 +1641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E455"/>
+  <dimension ref="A1:E469"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A455" sqref="A1:E455"/>
+    <sheetView tabSelected="1" topLeftCell="A443" workbookViewId="0">
+      <selection activeCell="D469" sqref="D469"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7225,6 +7279,202 @@
         <v>404</v>
       </c>
     </row>
+    <row r="456" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A456" t="s">
+        <v>29</v>
+      </c>
+      <c r="B456">
+        <v>20723</v>
+      </c>
+      <c r="C456" t="s">
+        <v>405</v>
+      </c>
+      <c r="D456" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A457" t="s">
+        <v>20</v>
+      </c>
+      <c r="B457">
+        <v>21147</v>
+      </c>
+      <c r="C457" t="s">
+        <v>405</v>
+      </c>
+      <c r="D457" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="458" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A458" t="s">
+        <v>20</v>
+      </c>
+      <c r="B458">
+        <v>21146</v>
+      </c>
+      <c r="C458" t="s">
+        <v>405</v>
+      </c>
+      <c r="D458" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A459" t="s">
+        <v>20</v>
+      </c>
+      <c r="B459">
+        <v>21148</v>
+      </c>
+      <c r="C459" t="s">
+        <v>405</v>
+      </c>
+      <c r="D459" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="460" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A460" t="s">
+        <v>20</v>
+      </c>
+      <c r="B460">
+        <v>21149</v>
+      </c>
+      <c r="C460" t="s">
+        <v>405</v>
+      </c>
+      <c r="D460" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A461" t="s">
+        <v>20</v>
+      </c>
+      <c r="B461">
+        <v>21150</v>
+      </c>
+      <c r="C461" t="s">
+        <v>405</v>
+      </c>
+      <c r="D461" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A462" t="s">
+        <v>20</v>
+      </c>
+      <c r="B462">
+        <v>21151</v>
+      </c>
+      <c r="C462" t="s">
+        <v>405</v>
+      </c>
+      <c r="D462" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="463" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A463" t="s">
+        <v>20</v>
+      </c>
+      <c r="B463">
+        <v>23637</v>
+      </c>
+      <c r="C463" t="s">
+        <v>405</v>
+      </c>
+      <c r="D463" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="464" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A464" t="s">
+        <v>20</v>
+      </c>
+      <c r="B464">
+        <v>23638</v>
+      </c>
+      <c r="C464" t="s">
+        <v>405</v>
+      </c>
+      <c r="D464" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A465" t="s">
+        <v>29</v>
+      </c>
+      <c r="B465">
+        <v>20723</v>
+      </c>
+      <c r="C465" t="s">
+        <v>414</v>
+      </c>
+      <c r="D465" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A466" t="s">
+        <v>7</v>
+      </c>
+      <c r="B466">
+        <v>22084</v>
+      </c>
+      <c r="C466" t="s">
+        <v>416</v>
+      </c>
+      <c r="D466" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A467" t="s">
+        <v>7</v>
+      </c>
+      <c r="B467">
+        <v>22085</v>
+      </c>
+      <c r="C467" t="s">
+        <v>416</v>
+      </c>
+      <c r="D467" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A468" t="s">
+        <v>29</v>
+      </c>
+      <c r="B468">
+        <v>24908</v>
+      </c>
+      <c r="C468" t="s">
+        <v>419</v>
+      </c>
+      <c r="D468" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A469" t="s">
+        <v>29</v>
+      </c>
+      <c r="B469">
+        <v>21346</v>
+      </c>
+      <c r="C469" t="s">
+        <v>421</v>
+      </c>
+      <c r="D469" t="s">
+        <v>422</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added info for dialog where you create and pick a project.
</commit_message>
<xml_diff>
--- a/Controls.xlsx
+++ b/Controls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl-Otto\Documents\src\NVDA\vismaadministration-nvdaaddon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A68E98-F1A6-4851-A5DF-1B0199E97BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5588F302-7541-4301-8A87-831A0A55C2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="1410" windowWidth="23040" windowHeight="12232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1747" yWindow="1747" windowWidth="23040" windowHeight="12233" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="441">
   <si>
     <t>WindowClassName</t>
   </si>
@@ -1324,6 +1324,60 @@
   </si>
   <si>
     <t>Fakturor</t>
+  </si>
+  <si>
+    <t>Transaktionstyp</t>
+  </si>
+  <si>
+    <t>Stafflingar</t>
+  </si>
+  <si>
+    <t>Hämta projekt</t>
+  </si>
+  <si>
+    <t>Projektnummer</t>
+  </si>
+  <si>
+    <t>Projektet startar</t>
+  </si>
+  <si>
+    <t>Projektet slutar</t>
+  </si>
+  <si>
+    <t>Kundnamn</t>
+  </si>
+  <si>
+    <t>Kundens ordernummer</t>
+  </si>
+  <si>
+    <t>Kontaktperson</t>
+  </si>
+  <si>
+    <t>Arbetsplats</t>
+  </si>
+  <si>
+    <t>Arbetsplats, fortsättning</t>
+  </si>
+  <si>
+    <t>Vårt ordernummer</t>
+  </si>
+  <si>
+    <t>Kontoplanstyp</t>
+  </si>
+  <si>
+    <t>Ansvarig</t>
+  </si>
+  <si>
+    <t>Anteckning 1</t>
+  </si>
+  <si>
+    <t>Anteckning 2</t>
+  </si>
+  <si>
+    <t>Anteckning 3</t>
+  </si>
+  <si>
+    <t>Anteckning 4</t>
   </si>
 </sst>
 </file>
@@ -1641,10 +1695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E469"/>
+  <dimension ref="A1:E491"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A443" workbookViewId="0">
-      <selection activeCell="D469" sqref="D469"/>
+    <sheetView tabSelected="1" topLeftCell="A465" workbookViewId="0">
+      <selection activeCell="B482" sqref="B482"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7475,6 +7529,314 @@
         <v>422</v>
       </c>
     </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A470" t="s">
+        <v>7</v>
+      </c>
+      <c r="B470">
+        <v>26662</v>
+      </c>
+      <c r="C470" t="s">
+        <v>247</v>
+      </c>
+      <c r="D470" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A471" t="s">
+        <v>29</v>
+      </c>
+      <c r="B471">
+        <v>21530</v>
+      </c>
+      <c r="C471" t="s">
+        <v>247</v>
+      </c>
+      <c r="D471" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A472" t="s">
+        <v>29</v>
+      </c>
+      <c r="B472">
+        <v>21521</v>
+      </c>
+      <c r="C472" t="s">
+        <v>247</v>
+      </c>
+      <c r="D472" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A473" t="s">
+        <v>7</v>
+      </c>
+      <c r="B473">
+        <v>22206</v>
+      </c>
+      <c r="C473" t="s">
+        <v>425</v>
+      </c>
+      <c r="D473" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A474" t="s">
+        <v>7</v>
+      </c>
+      <c r="B474">
+        <v>22207</v>
+      </c>
+      <c r="C474" t="s">
+        <v>425</v>
+      </c>
+      <c r="D474" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A475" t="s">
+        <v>7</v>
+      </c>
+      <c r="B475">
+        <v>22208</v>
+      </c>
+      <c r="C475" t="s">
+        <v>425</v>
+      </c>
+      <c r="D475" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A476" t="s">
+        <v>7</v>
+      </c>
+      <c r="B476">
+        <v>22209</v>
+      </c>
+      <c r="C476" t="s">
+        <v>425</v>
+      </c>
+      <c r="D476" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A477" t="s">
+        <v>7</v>
+      </c>
+      <c r="B477">
+        <v>22212</v>
+      </c>
+      <c r="C477" t="s">
+        <v>425</v>
+      </c>
+      <c r="D477" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A478" t="s">
+        <v>7</v>
+      </c>
+      <c r="B478">
+        <v>22213</v>
+      </c>
+      <c r="C478" t="s">
+        <v>425</v>
+      </c>
+      <c r="D478" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A479" t="s">
+        <v>7</v>
+      </c>
+      <c r="B479">
+        <v>22215</v>
+      </c>
+      <c r="C479" t="s">
+        <v>425</v>
+      </c>
+      <c r="D479" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="480" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A480" t="s">
+        <v>7</v>
+      </c>
+      <c r="B480">
+        <v>22216</v>
+      </c>
+      <c r="C480" t="s">
+        <v>425</v>
+      </c>
+      <c r="D480" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="481" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A481" t="s">
+        <v>7</v>
+      </c>
+      <c r="B481">
+        <v>22217</v>
+      </c>
+      <c r="C481" t="s">
+        <v>425</v>
+      </c>
+      <c r="D481" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="482" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A482" t="s">
+        <v>7</v>
+      </c>
+      <c r="B482">
+        <v>22218</v>
+      </c>
+      <c r="C482" t="s">
+        <v>425</v>
+      </c>
+      <c r="D482" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="483" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A483" t="s">
+        <v>7</v>
+      </c>
+      <c r="B483">
+        <v>22219</v>
+      </c>
+      <c r="C483" t="s">
+        <v>425</v>
+      </c>
+      <c r="D483" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="484" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A484" t="s">
+        <v>7</v>
+      </c>
+      <c r="B484">
+        <v>22220</v>
+      </c>
+      <c r="C484" t="s">
+        <v>425</v>
+      </c>
+      <c r="D484" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="485" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A485" t="s">
+        <v>7</v>
+      </c>
+      <c r="B485">
+        <v>22214</v>
+      </c>
+      <c r="C485" t="s">
+        <v>425</v>
+      </c>
+      <c r="D485" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="486" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A486" t="s">
+        <v>16</v>
+      </c>
+      <c r="B486">
+        <v>22225</v>
+      </c>
+      <c r="C486" t="s">
+        <v>425</v>
+      </c>
+      <c r="D486" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="487" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A487" t="s">
+        <v>7</v>
+      </c>
+      <c r="B487">
+        <v>22211</v>
+      </c>
+      <c r="C487" t="s">
+        <v>425</v>
+      </c>
+      <c r="D487" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="488" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A488" t="s">
+        <v>7</v>
+      </c>
+      <c r="B488">
+        <v>22221</v>
+      </c>
+      <c r="C488" t="s">
+        <v>425</v>
+      </c>
+      <c r="D488" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="489" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A489" t="s">
+        <v>7</v>
+      </c>
+      <c r="B489">
+        <v>22222</v>
+      </c>
+      <c r="C489" t="s">
+        <v>425</v>
+      </c>
+      <c r="D489" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="490" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A490" t="s">
+        <v>7</v>
+      </c>
+      <c r="B490">
+        <v>22223</v>
+      </c>
+      <c r="C490" t="s">
+        <v>425</v>
+      </c>
+      <c r="D490" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="491" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A491" t="s">
+        <v>7</v>
+      </c>
+      <c r="B491">
+        <v>22224</v>
+      </c>
+      <c r="C491" t="s">
+        <v>425</v>
+      </c>
+      <c r="D491" t="s">
+        <v>440</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>